<commit_message>
proj9.v1.5:Wszystko ukończone poza pbh
</commit_message>
<xml_diff>
--- a/database/ml_projekty.xlsx
+++ b/database/ml_projekty.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\repos\MECHANIKA_LOTU\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0FC69F-F79E-4DB4-B104-48A49D36565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFB0C48-D560-4A33-8631-C58953C4FC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45960" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="10" r:id="rId1"/>
-    <sheet name="Dane proj2_copy" sheetId="1" r:id="rId2"/>
+    <sheet name="proj2_copy" sheetId="1" r:id="rId2"/>
     <sheet name="Base" sheetId="3" r:id="rId3"/>
     <sheet name="proj3" sheetId="2" r:id="rId4"/>
     <sheet name="proj4" sheetId="4" r:id="rId5"/>
@@ -93,8 +93,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="348">
   <si>
     <t>Co liczę</t>
   </si>
@@ -1009,9 +1031,6 @@
     <t>Kappa3</t>
   </si>
   <si>
-    <t>Lambda_H</t>
-  </si>
-  <si>
     <t>b_h</t>
   </si>
   <si>
@@ -1029,6 +1048,135 @@
   <si>
     <t>Lambda_h</t>
   </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>SsH</t>
+  </si>
+  <si>
+    <t>deps_dalpha</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>xc</t>
+  </si>
+  <si>
+    <t>Cmbu</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>azh [rad]</t>
+  </si>
+  <si>
+    <t>azh [deg]</t>
+  </si>
+  <si>
+    <t>Wyznaczanie azh - kąta zaklinowania płata</t>
+  </si>
+  <si>
+    <t>&lt;- powierzchnia steru</t>
+  </si>
+  <si>
+    <t>śr.c_h</t>
+  </si>
+  <si>
+    <t>&lt;- wzór na środek cięzkości trapezu</t>
+  </si>
+  <si>
+    <t>stosunek średniej cięciwy części steru przed osią obrotu do średniej cięciwy całego steru</t>
+  </si>
+  <si>
+    <t>csh</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>śr.c_sh</t>
+  </si>
+  <si>
+    <t>c_sh1</t>
+  </si>
+  <si>
+    <t>c_sh2</t>
+  </si>
+  <si>
+    <t>csh/ch</t>
+  </si>
+  <si>
+    <t>ckh</t>
+  </si>
+  <si>
+    <t>ckh/csh</t>
+  </si>
+  <si>
+    <t>Odczyty z tabelek (9.2) - b_3 inf</t>
+  </si>
+  <si>
+    <t>śr</t>
+  </si>
+  <si>
+    <t>b3_inf</t>
+  </si>
+  <si>
+    <t>a1inf</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b1inf</t>
+  </si>
+  <si>
+    <t>b2inf</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>eta_sh</t>
+  </si>
+  <si>
+    <t>k_kl</t>
+  </si>
+  <si>
+    <t>b_kh</t>
+  </si>
+  <si>
+    <t>S_kh</t>
+  </si>
+  <si>
+    <t>śr.c_kh</t>
+  </si>
+  <si>
+    <t>S0_kh</t>
+  </si>
+  <si>
+    <t>eta_skH</t>
+  </si>
+  <si>
+    <t>Ssh/Sh</t>
+  </si>
+  <si>
+    <t>Skh/Ssh</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>przelicznik</t>
+  </si>
+  <si>
+    <t>b3inf</t>
+  </si>
 </sst>
 </file>
 
@@ -1040,7 +1188,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1209,6 +1357,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1285,13 +1440,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="2" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1406,7 +1561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1528,10 +1683,14 @@
     <xf numFmtId="164" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1577,8 +1736,16 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1866,10 +2033,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2724150" cy="2952750"/>
     <xdr:pic>
@@ -1891,7 +2058,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5657850" y="1749425"/>
+          <a:off x="12979400" y="3654425"/>
           <a:ext cx="2724150" cy="2952750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1904,10 +2071,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>73025</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4200525" cy="438150"/>
     <xdr:pic>
@@ -1928,6 +2095,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10398125" y="4254500"/>
+          <a:ext cx="4200525" cy="438150"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1938,9 +2109,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5362575" cy="523875"/>
@@ -1962,6 +2133,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10115550" y="4933950"/>
+          <a:ext cx="5362575" cy="523875"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1970,6 +2145,275 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419893</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>56752</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>387768</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>55254</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1" descr="Obraz zawierający Czcionka, tekst, biały, kaligrafia&#10;&#10;Opis wygenerowany automatycznie">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7094CF07-702E-D8BA-4F14-E6BAF581361F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6855221" y="699690"/>
+          <a:ext cx="3000794" cy="641439"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>15081</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>125412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>145614</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>102900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Obraz 2" descr="Obraz zawierający Czcionka, linia, numer, biały&#10;&#10;Opis wygenerowany automatycznie">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7974F1A-C294-EFA5-921F-B3900EEBEC04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7057628" y="1411287"/>
+          <a:ext cx="2556233" cy="784335"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>115094</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>219617</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>189099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obraz 3" descr="Obraz zawierający Czcionka, tekst, linia, biały&#10;&#10;Opis wygenerowany automatycznie">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7A8A3FF-2FB7-1893-BCF9-E5FC1C44B810}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7080250" y="2353469"/>
+          <a:ext cx="3889917" cy="865313"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>388937</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>121687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>292893</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>141512</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Obraz 4" descr="Obraz zawierający tekst, zrzut ekranu, Czcionka, linia&#10;&#10;Opis wygenerowany automatycznie">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{232ED540-CFD7-76B0-7D2C-CF97BDE16FA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3159125" y="3947562"/>
+          <a:ext cx="3599656" cy="975501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>325437</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>146843</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>277976</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>64414</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Obraz 5" descr="Obraz zawierający Czcionka, tekst, linia, zrzut ekranu&#10;&#10;Opis wygenerowany automatycznie">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E03D2EA2-C608-34E0-D853-38EA85FB1237}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7469187" y="5091906"/>
+          <a:ext cx="1171739" cy="866896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276609</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Obraz 6" descr="Obraz zawierający tekst, Czcionka, linia, biały&#10;&#10;Opis wygenerowany automatycznie">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACED6C21-D0C4-B8EA-38FE-1C43923CB368}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2820865" y="7253654"/>
+          <a:ext cx="2735281" cy="746471"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2202,14 +2646,14 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="26" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -36444,43 +36888,43 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.90625" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
     <col min="2" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="23"/>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="89" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="85" t="s">
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="89" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="85" t="s">
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="89" t="s">
         <v>166</v>
       </c>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92" t="s">
         <v>167</v>
       </c>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
+      <c r="S1" s="93"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="93"/>
+      <c r="V1" s="93"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="39" t="s">
@@ -38847,14 +39291,14 @@
       <selection activeCell="A30" sqref="A30:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
     <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="6.54296875" customWidth="1"/>
     <col min="6" max="6" width="23.7265625" customWidth="1"/>
-    <col min="7" max="7" width="20.90625" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="10" max="10" width="7.7265625" customWidth="1"/>
   </cols>
@@ -38991,7 +39435,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="13">
-      <c r="A8" s="92" t="s">
+      <c r="A8" s="96" t="s">
         <v>86</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -39009,7 +39453,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A9" s="91"/>
+      <c r="A9" s="95"/>
       <c r="B9" s="6" t="s">
         <v>89</v>
       </c>
@@ -39030,7 +39474,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A10" s="91"/>
+      <c r="A10" s="95"/>
       <c r="B10" s="21" t="s">
         <v>92</v>
       </c>
@@ -39048,7 +39492,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A11" s="91"/>
+      <c r="A11" s="95"/>
       <c r="B11" s="21" t="s">
         <v>95</v>
       </c>
@@ -39099,14 +39543,14 @@
       <c r="B18" s="6">
         <v>1.5</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="87"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="91"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="6" t="s">
@@ -39383,10 +39827,10 @@
         <f>0.355/B18</f>
         <v>0.23666666666666666</v>
       </c>
-      <c r="E32" s="94" t="s">
+      <c r="E32" s="98" t="s">
         <v>134</v>
       </c>
-      <c r="F32" s="91"/>
+      <c r="F32" s="95"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="21" t="s">
@@ -39436,10 +39880,10 @@
         <f>1/B35*(B27+B33*(B31-B32))</f>
         <v>-0.10312152368291011</v>
       </c>
-      <c r="E37" s="95" t="s">
+      <c r="E37" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="F37" s="91"/>
+      <c r="F37" s="95"/>
     </row>
     <row r="38" spans="1:6" ht="15.5">
       <c r="E38" s="6" t="s">
@@ -39498,10 +39942,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="13">
-      <c r="A48" s="90" t="s">
+      <c r="A48" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="B48" s="91"/>
+      <c r="B48" s="95"/>
     </row>
     <row r="49" spans="1:3" ht="12.5">
       <c r="A49" s="6" t="s">
@@ -39548,10 +39992,10 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="13">
-      <c r="A55" s="90" t="s">
+      <c r="A55" s="94" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="91"/>
+      <c r="B55" s="95"/>
     </row>
     <row r="56" spans="1:3" ht="12.5">
       <c r="A56" s="6" t="s">
@@ -39563,10 +40007,10 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="13">
-      <c r="A58" s="90" t="s">
+      <c r="A58" s="94" t="s">
         <v>156</v>
       </c>
-      <c r="B58" s="91"/>
+      <c r="B58" s="95"/>
     </row>
     <row r="59" spans="1:3" ht="12.5">
       <c r="A59" s="6" t="s">
@@ -39661,11 +40105,11 @@
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.453125" customWidth="1"/>
     <col min="2" max="2" width="7.26953125" customWidth="1"/>
-    <col min="9" max="19" width="8.08984375" customWidth="1"/>
+    <col min="9" max="19" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="13">
@@ -39675,33 +40119,33 @@
       <c r="B1" s="6">
         <v>600</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="I1" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="99" t="s">
+      <c r="J1" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="99" t="s">
+      <c r="K1" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="99" t="s">
+      <c r="L1" s="103" t="s">
         <v>173</v>
       </c>
-      <c r="M1" s="99" t="s">
+      <c r="M1" s="103" t="s">
         <v>170</v>
       </c>
-      <c r="N1" s="96" t="s">
+      <c r="N1" s="100" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="91"/>
-      <c r="P1" s="97" t="s">
+      <c r="O1" s="95"/>
+      <c r="P1" s="101" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="97" t="s">
+      <c r="Q1" s="95"/>
+      <c r="R1" s="101" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="91"/>
+      <c r="S1" s="95"/>
     </row>
     <row r="2" spans="1:19" ht="13">
       <c r="A2" s="21" t="s">
@@ -39710,11 +40154,11 @@
       <c r="B2" s="6">
         <v>726</v>
       </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
       <c r="N2" s="41" t="s">
         <v>178</v>
       </c>
@@ -39938,7 +40382,7 @@
         <v>2.9154578604593531</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="39.5" customHeight="1">
+    <row r="7" spans="1:19" ht="39.65" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>188</v>
       </c>
@@ -40035,15 +40479,15 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="13">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="94" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="91"/>
-      <c r="D9" s="90" t="s">
+      <c r="B9" s="95"/>
+      <c r="D9" s="94" t="s">
         <v>190</v>
       </c>
-      <c r="E9" s="91"/>
-      <c r="F9" s="91"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
       <c r="I9" s="42">
         <v>1.5</v>
       </c>
@@ -40632,7 +41076,7 @@
       </c>
     </row>
     <row r="20" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="102" t="s">
         <v>203</v>
       </c>
       <c r="C20" s="49" t="s">
@@ -40698,7 +41142,7 @@
       </c>
     </row>
     <row r="21" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B21" s="91"/>
+      <c r="B21" s="95"/>
       <c r="C21" s="49" t="s">
         <v>205</v>
       </c>
@@ -40762,7 +41206,7 @@
       </c>
     </row>
     <row r="22" spans="2:21" ht="13">
-      <c r="B22" s="91"/>
+      <c r="B22" s="95"/>
       <c r="C22" s="49" t="s">
         <v>206</v>
       </c>
@@ -40830,7 +41274,7 @@
       </c>
     </row>
     <row r="23" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B23" s="91"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="49" t="s">
         <v>207</v>
       </c>
@@ -40897,7 +41341,7 @@
       </c>
     </row>
     <row r="24" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="102" t="s">
         <v>208</v>
       </c>
       <c r="C24" s="49" t="s">
@@ -40966,7 +41410,7 @@
       </c>
     </row>
     <row r="25" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B25" s="91"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="49" t="s">
         <v>205</v>
       </c>
@@ -41033,7 +41477,7 @@
       </c>
     </row>
     <row r="26" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B26" s="91"/>
+      <c r="B26" s="95"/>
       <c r="C26" s="49" t="s">
         <v>206</v>
       </c>
@@ -41100,7 +41544,7 @@
       </c>
     </row>
     <row r="27" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B27" s="91"/>
+      <c r="B27" s="95"/>
       <c r="C27" s="49" t="s">
         <v>207</v>
       </c>
@@ -41167,7 +41611,7 @@
       </c>
     </row>
     <row r="28" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B28" s="98" t="s">
+      <c r="B28" s="102" t="s">
         <v>209</v>
       </c>
       <c r="C28" s="49" t="s">
@@ -41233,7 +41677,7 @@
       </c>
     </row>
     <row r="29" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B29" s="91"/>
+      <c r="B29" s="95"/>
       <c r="C29" s="49" t="s">
         <v>205</v>
       </c>
@@ -41297,7 +41741,7 @@
       </c>
     </row>
     <row r="30" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B30" s="91"/>
+      <c r="B30" s="95"/>
       <c r="C30" s="49" t="s">
         <v>206</v>
       </c>
@@ -41361,7 +41805,7 @@
       </c>
     </row>
     <row r="31" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B31" s="91"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="49" t="s">
         <v>207</v>
       </c>
@@ -54245,26 +54689,26 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.08984375" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
     <col min="2" max="2" width="7.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
     <col min="4" max="4" width="7.453125" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="7.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="104" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
     </row>
     <row r="2" spans="1:12" ht="13">
       <c r="A2" s="57" t="s">
@@ -54366,12 +54810,12 @@
       <c r="D7" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="98" t="s">
         <v>230</v>
       </c>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="F8" s="6" t="s">
@@ -54806,26 +55250,26 @@
   <dimension ref="A1:S1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C10"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="7" max="7" width="9.26953125" customWidth="1"/>
-    <col min="8" max="8" width="5.36328125" customWidth="1"/>
+    <col min="8" max="8" width="5.453125" customWidth="1"/>
     <col min="9" max="9" width="6.26953125" customWidth="1"/>
-    <col min="10" max="19" width="8.6328125" customWidth="1"/>
+    <col min="10" max="19" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="13">
       <c r="C1" s="66"/>
       <c r="H1" s="23"/>
-      <c r="I1" s="101" t="s">
+      <c r="I1" s="105" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="87"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="87"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="91"/>
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
@@ -54837,7 +55281,7 @@
       <c r="R1" s="19"/>
       <c r="S1" s="19"/>
     </row>
-    <row r="2" spans="1:19" ht="15.5" customHeight="1">
+    <row r="2" spans="1:19" ht="15.65" customHeight="1">
       <c r="B2" s="6" t="s">
         <v>255</v>
       </c>
@@ -54979,7 +55423,7 @@
         <v>-0.11743541308971617</v>
       </c>
       <c r="P4" s="73">
-        <f t="shared" si="3"/>
+        <f>$G$2 + J4*$C$17-(K4- L4*PI()/180*J4)*$C$13</f>
         <v>-0.23274614755299289</v>
       </c>
       <c r="Q4" s="73">
@@ -70406,7 +70850,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -72091,167 +72535,654 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED024D9D-FA85-4F12-A2B8-B7F640D257BC}">
   <sheetPr codeName="Arkusz9"/>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="84" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13">
-      <c r="A1" s="103" t="s">
+    <row r="1" spans="1:8" ht="13">
+      <c r="A1" s="107" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="D1" s="104" t="s">
+      <c r="B1" s="107"/>
+      <c r="D1" s="108" t="s">
         <v>295</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="19">
         <v>0.85</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="81" t="s">
         <v>271</v>
       </c>
-      <c r="E2" s="83">
+      <c r="E2" s="82">
         <v>0.12</v>
       </c>
       <c r="F2" s="80" t="s">
         <v>296</v>
       </c>
-      <c r="G2" s="84">
+      <c r="G2" s="83">
         <f xml:space="preserve"> (B$5 - E2)*B$3/B$4 *B$2</f>
         <v>0.34255075555555559</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="80" t="s">
         <v>292</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="84">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="81" t="s">
         <v>272</v>
       </c>
-      <c r="E3" s="83">
+      <c r="E3" s="82">
         <v>0.25</v>
       </c>
       <c r="F3" s="80" t="s">
         <v>297</v>
       </c>
-      <c r="G3" s="84">
+      <c r="G3" s="83">
         <f xml:space="preserve"> (B$5 - E3)*B$3/B$4 *B$2</f>
         <v>0.32634408888888894</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="80" t="s">
         <v>293</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="84">
         <v>15</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="81" t="s">
         <v>273</v>
       </c>
-      <c r="E4" s="83">
+      <c r="E4" s="82">
         <v>0.38</v>
       </c>
       <c r="F4" s="80" t="s">
         <v>298</v>
       </c>
-      <c r="G4" s="84">
+      <c r="G4" s="83">
         <f xml:space="preserve"> (B$5 - E4)*B$3/B$4 *B$2</f>
         <v>0.31013742222222229</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="80" t="s">
         <v>291</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="84">
         <f xml:space="preserve"> 8*53.77/150</f>
         <v>2.8677333333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="6" spans="1:8" ht="13">
+      <c r="D6" s="108" t="s">
+        <v>315</v>
+      </c>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="C7" s="80"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="80" t="s">
+      <c r="D7" s="86" t="s">
+        <v>310</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>311</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>312</v>
+      </c>
+      <c r="G7" s="86" t="s">
+        <v>313</v>
+      </c>
+      <c r="H7" s="86" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>299</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B8" s="84">
+        <v>3.01</v>
+      </c>
+      <c r="D8" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="E8" s="87" cm="1">
+        <f t="array" ref="E8:E10" xml:space="preserve"> TRANSPOSE(proj8!Q22:S22)</f>
+        <v>-7.4770965467342465E-2</v>
+      </c>
+      <c r="F8" s="88" cm="1">
+        <f t="array" ref="F8:F10" xml:space="preserve"> G2:G4</f>
+        <v>0.34255075555555559</v>
+      </c>
+      <c r="G8" s="87">
+        <f xml:space="preserve"> E8/(F8*$B$33)-$B$36/$B$31*(1-$B$37)</f>
+        <v>-0.10396623227262985</v>
+      </c>
+      <c r="H8" s="87">
+        <f xml:space="preserve"> DEGREES(G8)</f>
+        <v>-5.9568263210985037</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>300</v>
       </c>
-      <c r="E11">
-        <v>3.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="D12" t="s">
-        <v>301</v>
-      </c>
-      <c r="E12">
+      <c r="B9" s="84">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="D13" t="s">
-        <v>303</v>
-      </c>
-      <c r="E13">
+      <c r="D9" s="82">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="87">
+        <v>-3.9516728179206879E-2</v>
+      </c>
+      <c r="F9" s="87">
+        <v>0.32634408888888894</v>
+      </c>
+      <c r="G9" s="87">
+        <f xml:space="preserve"> E9/(F9*$B$33)-$B$36/$B$31*(1-$B$37)</f>
+        <v>-7.2615299398383903E-2</v>
+      </c>
+      <c r="H9" s="87">
+        <f xml:space="preserve"> DEGREES(G9)</f>
+        <v>-4.1605501836062633</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B10" s="84">
         <f xml:space="preserve"> 1.4*52.11/100</f>
         <v>0.72953999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="D14" t="s">
-        <v>304</v>
-      </c>
-      <c r="E14">
+      <c r="D10" s="82">
+        <v>0.38</v>
+      </c>
+      <c r="E10" s="87">
+        <v>-4.2624908910712939E-3</v>
+      </c>
+      <c r="F10" s="87">
+        <v>0.31013742222222229</v>
+      </c>
+      <c r="G10" s="87">
+        <f xml:space="preserve"> E10/(F10*$B$33)-$B$36/$B$31*(1-$B$37)</f>
+        <v>-3.7987792448418198E-2</v>
+      </c>
+      <c r="H10" s="87">
+        <f t="shared" ref="H10" si="0" xml:space="preserve"> DEGREES(G10)</f>
+        <v>-2.1765401803133027</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" s="84">
         <f xml:space="preserve"> 2.1*52.11/100</f>
         <v>1.0943099999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="D15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E15">
-        <f>1/(E14/E13)</f>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>317</v>
+      </c>
+      <c r="B12" s="84">
+        <f>B8/(2*3)*(2*B11+B10)/(B11+B10)</f>
+        <v>0.80266666666666664</v>
+      </c>
+      <c r="C12" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" s="84">
+        <f>0.5*52.11/100</f>
+        <v>0.26055</v>
+      </c>
+      <c r="C13" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>324</v>
+      </c>
+      <c r="B14" s="84">
+        <f>0.9*52.11/100</f>
+        <v>0.46899000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B15" s="84">
+        <f xml:space="preserve"> 1/3*(2*B13+B14)/(B13+B14)</f>
+        <v>0.45238095238095233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="80" t="s">
+        <v>340</v>
+      </c>
+      <c r="B16" s="84">
+        <f>0.3*52.11/100</f>
+        <v>0.15633</v>
+      </c>
+      <c r="F16" s="80"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="80" t="s">
+        <v>338</v>
+      </c>
+      <c r="B17" s="111">
+        <f>3.1*52.11/100</f>
+        <v>1.61541</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="str" cm="1">
+        <f t="array" ref="A18:B19" xml:space="preserve"> F37:G38</f>
+        <v>S_kh</v>
+      </c>
+      <c r="B18" s="84">
+        <v>0.25253704529999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" t="str">
+        <v>S0_kh</v>
+      </c>
+      <c r="B19" s="84">
+        <v>0.47055329999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="26" customHeight="1">
+      <c r="A20" s="80" t="s">
+        <v>337</v>
+      </c>
+      <c r="B20" s="84">
+        <f xml:space="preserve"> (B18*B17)/(B19*B8)</f>
+        <v>0.28802656351475153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
+        <v>301</v>
+      </c>
+      <c r="B22" s="84">
+        <f>1/(B11/B10)</f>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="D16" t="s">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" t="s">
+        <v>304</v>
+      </c>
+      <c r="B23" s="84">
+        <f xml:space="preserve"> B8^2/B9</f>
+        <v>4.118227272727272</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:17" ht="13">
+      <c r="A25" s="80" t="s">
+        <v>309</v>
+      </c>
+      <c r="B25" s="112">
+        <f>proj2_copy!H9</f>
+        <v>6.5967841001666665</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="110" t="s">
+        <v>328</v>
+      </c>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="110"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="s">
+        <v>307</v>
+      </c>
+      <c r="B26" s="84">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="C26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="87" t="s">
+        <v>320</v>
+      </c>
+      <c r="G26" s="109">
+        <f>B15</f>
+        <v>0.45238095238095233</v>
+      </c>
+      <c r="H26" s="87" t="s">
+        <v>326</v>
+      </c>
+      <c r="I26" s="109">
+        <f>B16</f>
+        <v>0.15633</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="80" t="s">
+        <v>343</v>
+      </c>
+      <c r="B27" s="84">
+        <f xml:space="preserve"> B26/B3</f>
+        <v>0.42454545454545456</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="87" t="s">
+        <v>321</v>
+      </c>
+      <c r="G27" s="109">
+        <f>B12</f>
+        <v>0.80266666666666664</v>
+      </c>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="80" t="s">
+        <v>344</v>
+      </c>
+      <c r="B28" s="84">
+        <f xml:space="preserve"> B18/B26</f>
+        <v>0.27038227548179866</v>
+      </c>
+      <c r="F28" s="87" t="s">
+        <v>325</v>
+      </c>
+      <c r="G28" s="87">
+        <f>G26/G27</f>
+        <v>0.56359753203607021</v>
+      </c>
+      <c r="H28" s="87" t="s">
+        <v>327</v>
+      </c>
+      <c r="I28" s="87">
+        <f>I26/G26</f>
+        <v>0.34557157894736845</v>
+      </c>
+      <c r="K28" s="80" t="s">
+        <v>330</v>
+      </c>
+      <c r="L28">
+        <f>-0.025</f>
+        <v>-2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="P30" s="80" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="84">
+        <f>proj2_copy!H37</f>
+        <v>4.4523373266764565</v>
+      </c>
+      <c r="M31">
+        <v>0.1</v>
+      </c>
+      <c r="N31" s="80">
+        <v>-1.0749999999999999E-2</v>
+      </c>
+      <c r="O31" s="80">
+        <v>-1.0749999999999999E-2</v>
+      </c>
+      <c r="P31">
+        <f>AVERAGE(N31:O31)</f>
+        <v>-1.0749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="B32" s="85"/>
+      <c r="M32">
+        <v>0.2</v>
+      </c>
+      <c r="N32">
+        <v>-1.5800000000000002E-2</v>
+      </c>
+      <c r="O32" s="80">
+        <v>-1.6750000000000001E-2</v>
+      </c>
+      <c r="P32">
+        <f t="shared" ref="P32:P33" si="1">AVERAGE(N32:O32)</f>
+        <v>-1.6275000000000001E-2</v>
+      </c>
+      <c r="Q32">
+        <f xml:space="preserve"> P32-P31</f>
+        <v>-5.5250000000000021E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" t="s">
         <v>305</v>
       </c>
-      <c r="E16">
-        <f xml:space="preserve"> E11^2/E12</f>
-        <v>4.118227272727272</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="81"/>
-      <c r="B18" s="81"/>
+      <c r="B33" s="84">
+        <v>3.1</v>
+      </c>
+      <c r="M33">
+        <v>0.3</v>
+      </c>
+      <c r="N33" s="80">
+        <v>-1.9199999999999998E-2</v>
+      </c>
+      <c r="O33" s="80">
+        <v>-0.02</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>-1.9599999999999999E-2</v>
+      </c>
+      <c r="Q33">
+        <f xml:space="preserve"> P33-P32</f>
+        <v>-3.3249999999999981E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" s="80" t="s">
+        <v>331</v>
+      </c>
+      <c r="B34" s="84">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="M34">
+        <v>0.35</v>
+      </c>
+      <c r="P34">
+        <v>-3.2099999999999997E-2</v>
+      </c>
+      <c r="Q34">
+        <f xml:space="preserve"> P34-P33</f>
+        <v>-1.2499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" t="s">
+        <v>306</v>
+      </c>
+      <c r="B35" s="84">
+        <f xml:space="preserve"> 1.2*B33*SQRT(B27)*(1-0.2*B27)</f>
+        <v>2.2180395125888839</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" s="80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="84">
+        <f xml:space="preserve"> 2*726*9.81/(1.225*15*54.4^2)</f>
+        <v>0.2619452192641763</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" s="80" t="s">
+        <v>308</v>
+      </c>
+      <c r="B37" s="84">
+        <f xml:space="preserve"> 2*B31/(PI()*B25)</f>
+        <v>0.42967087180264696</v>
+      </c>
+      <c r="F37" s="80" t="s">
+        <v>339</v>
+      </c>
+      <c r="G37">
+        <f xml:space="preserve"> B17*B16</f>
+        <v>0.25253704529999998</v>
+      </c>
+      <c r="J37" s="80"/>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="F38" s="80" t="s">
+        <v>341</v>
+      </c>
+      <c r="G38">
+        <f>B8*B16</f>
+        <v>0.47055329999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="80" t="s">
+        <v>333</v>
+      </c>
+      <c r="B39" s="84">
+        <f>C39*E42</f>
+        <v>-1.4323944878270582</v>
+      </c>
+      <c r="C39">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="F39" s="80" t="s">
+        <v>337</v>
+      </c>
+      <c r="G39">
+        <f xml:space="preserve"> (G37*B17)/(G38*B8)</f>
+        <v>0.28802656351475153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="80" t="s">
+        <v>332</v>
+      </c>
+      <c r="B40" s="84">
+        <f xml:space="preserve"> B39*B33/B34</f>
+        <v>-0.90620875760487352</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" s="80" t="s">
+        <v>342</v>
+      </c>
+      <c r="B42" s="84">
+        <v>0.47</v>
+      </c>
+      <c r="D42" s="80" t="s">
+        <v>346</v>
+      </c>
+      <c r="E42">
+        <f>180/PI()</f>
+        <v>57.295779513082323</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" s="80" t="s">
+        <v>336</v>
+      </c>
+      <c r="B43" s="84">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" s="80" t="s">
+        <v>334</v>
+      </c>
+      <c r="B44" s="84">
+        <f>C44*E42</f>
+        <v>-0.35408791739084872</v>
+      </c>
+      <c r="C44">
+        <v>-6.1799999999999997E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45" s="80" t="s">
+        <v>335</v>
+      </c>
+      <c r="B45" s="84">
+        <f xml:space="preserve"> B44+(B33/B34-1)*B40*B43</f>
+        <v>-0.15435210959222351</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" s="80" t="s">
+        <v>347</v>
+      </c>
+      <c r="B47" s="84">
+        <f xml:space="preserve"> C47*E42</f>
+        <v>-1.4323944878270582</v>
+      </c>
+      <c r="C47">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="B48" s="84">
+        <f xml:space="preserve"> B47*B20-(B33/B34-1)*B40*B42</f>
+        <v>-0.5690273780352233</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="F25:I25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
proj9.v1:Final version with excel
</commit_message>
<xml_diff>
--- a/database/ml_projekty.xlsx
+++ b/database/ml_projekty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\repos\MECHANIKA_LOTU\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFB0C48-D560-4A33-8631-C58953C4FC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17F0D6C-F3B3-4AFD-83A0-1D8903960855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45960" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,6 +56,8 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="238"/>
             <scheme val="minor"/>
           </rPr>
           <t>dla kąta natarcia = -1 deg
@@ -82,6 +84,8 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="238"/>
             <scheme val="minor"/>
           </rPr>
           <t>nie jestem pewien, nie wiem skąd wziąć z_c nigdzie w projektach nie było liczone
@@ -116,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="351">
   <si>
     <t>Co liczę</t>
   </si>
@@ -1177,6 +1181,15 @@
   <si>
     <t>b3inf</t>
   </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>cz(v)</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
 </sst>
 </file>
 
@@ -1199,17 +1212,23 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1221,11 +1240,15 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFADBAC7"/>
       <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1237,33 +1260,45 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1275,16 +1310,22 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1292,11 +1333,15 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
@@ -1304,12 +1349,16 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="17"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1561,7 +1610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1691,6 +1740,19 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1739,13 +1801,8 @@
     <xf numFmtId="0" fontId="28" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2159,7 +2216,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>387768</xdr:colOff>
+      <xdr:colOff>390943</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>55254</xdr:rowOff>
     </xdr:to>
@@ -2203,9 +2260,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>145614</xdr:colOff>
+      <xdr:colOff>142439</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>102900</xdr:rowOff>
+      <xdr:rowOff>106075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2247,7 +2304,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>219617</xdr:colOff>
+      <xdr:colOff>216442</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>189099</xdr:rowOff>
     </xdr:to>
@@ -2291,9 +2348,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>292893</xdr:colOff>
+      <xdr:colOff>296068</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>141512</xdr:rowOff>
+      <xdr:rowOff>144687</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2335,9 +2392,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>277976</xdr:colOff>
+      <xdr:colOff>274801</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>64414</xdr:rowOff>
+      <xdr:rowOff>67589</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2379,9 +2436,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>276609</xdr:colOff>
+      <xdr:colOff>273434</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>104877</xdr:rowOff>
+      <xdr:rowOff>101702</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -36896,35 +36953,35 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="23"/>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="96" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="89" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="89" t="s">
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="96" t="s">
         <v>166</v>
       </c>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="92" t="s">
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="99" t="s">
         <v>167</v>
       </c>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="39" t="s">
@@ -39435,7 +39492,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="13">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="103" t="s">
         <v>86</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -39453,7 +39510,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A9" s="95"/>
+      <c r="A9" s="102"/>
       <c r="B9" s="6" t="s">
         <v>89</v>
       </c>
@@ -39474,7 +39531,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A10" s="95"/>
+      <c r="A10" s="102"/>
       <c r="B10" s="21" t="s">
         <v>92</v>
       </c>
@@ -39492,7 +39549,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A11" s="95"/>
+      <c r="A11" s="102"/>
       <c r="B11" s="21" t="s">
         <v>95</v>
       </c>
@@ -39543,14 +39600,14 @@
       <c r="B18" s="6">
         <v>1.5</v>
       </c>
-      <c r="E18" s="97" t="s">
+      <c r="E18" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="91"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="98"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="6" t="s">
@@ -39827,10 +39884,10 @@
         <f>0.355/B18</f>
         <v>0.23666666666666666</v>
       </c>
-      <c r="E32" s="98" t="s">
+      <c r="E32" s="105" t="s">
         <v>134</v>
       </c>
-      <c r="F32" s="95"/>
+      <c r="F32" s="102"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="21" t="s">
@@ -39880,10 +39937,10 @@
         <f>1/B35*(B27+B33*(B31-B32))</f>
         <v>-0.10312152368291011</v>
       </c>
-      <c r="E37" s="99" t="s">
+      <c r="E37" s="106" t="s">
         <v>141</v>
       </c>
-      <c r="F37" s="95"/>
+      <c r="F37" s="102"/>
     </row>
     <row r="38" spans="1:6" ht="15.5">
       <c r="E38" s="6" t="s">
@@ -39942,10 +39999,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="13">
-      <c r="A48" s="94" t="s">
+      <c r="A48" s="101" t="s">
         <v>149</v>
       </c>
-      <c r="B48" s="95"/>
+      <c r="B48" s="102"/>
     </row>
     <row r="49" spans="1:3" ht="12.5">
       <c r="A49" s="6" t="s">
@@ -39992,10 +40049,10 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="13">
-      <c r="A55" s="94" t="s">
+      <c r="A55" s="101" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="95"/>
+      <c r="B55" s="102"/>
     </row>
     <row r="56" spans="1:3" ht="12.5">
       <c r="A56" s="6" t="s">
@@ -40007,10 +40064,10 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="13">
-      <c r="A58" s="94" t="s">
+      <c r="A58" s="101" t="s">
         <v>156</v>
       </c>
-      <c r="B58" s="95"/>
+      <c r="B58" s="102"/>
     </row>
     <row r="59" spans="1:3" ht="12.5">
       <c r="A59" s="6" t="s">
@@ -40119,33 +40176,33 @@
       <c r="B1" s="6">
         <v>600</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="103" t="s">
+      <c r="J1" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="103" t="s">
+      <c r="K1" s="110" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="L1" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="M1" s="103" t="s">
+      <c r="M1" s="110" t="s">
         <v>170</v>
       </c>
-      <c r="N1" s="100" t="s">
+      <c r="N1" s="107" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="95"/>
-      <c r="P1" s="101" t="s">
+      <c r="O1" s="102"/>
+      <c r="P1" s="108" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="101" t="s">
+      <c r="Q1" s="102"/>
+      <c r="R1" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="95"/>
+      <c r="S1" s="102"/>
     </row>
     <row r="2" spans="1:19" ht="13">
       <c r="A2" s="21" t="s">
@@ -40154,11 +40211,11 @@
       <c r="B2" s="6">
         <v>726</v>
       </c>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
       <c r="N2" s="41" t="s">
         <v>178</v>
       </c>
@@ -40479,15 +40536,15 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="13">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="101" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="95"/>
-      <c r="D9" s="94" t="s">
+      <c r="B9" s="102"/>
+      <c r="D9" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
       <c r="I9" s="42">
         <v>1.5</v>
       </c>
@@ -41076,7 +41133,7 @@
       </c>
     </row>
     <row r="20" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B20" s="102" t="s">
+      <c r="B20" s="109" t="s">
         <v>203</v>
       </c>
       <c r="C20" s="49" t="s">
@@ -41142,7 +41199,7 @@
       </c>
     </row>
     <row r="21" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B21" s="95"/>
+      <c r="B21" s="102"/>
       <c r="C21" s="49" t="s">
         <v>205</v>
       </c>
@@ -41206,7 +41263,7 @@
       </c>
     </row>
     <row r="22" spans="2:21" ht="13">
-      <c r="B22" s="95"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="49" t="s">
         <v>206</v>
       </c>
@@ -41274,7 +41331,7 @@
       </c>
     </row>
     <row r="23" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B23" s="95"/>
+      <c r="B23" s="102"/>
       <c r="C23" s="49" t="s">
         <v>207</v>
       </c>
@@ -41341,7 +41398,7 @@
       </c>
     </row>
     <row r="24" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B24" s="102" t="s">
+      <c r="B24" s="109" t="s">
         <v>208</v>
       </c>
       <c r="C24" s="49" t="s">
@@ -41410,7 +41467,7 @@
       </c>
     </row>
     <row r="25" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B25" s="95"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="49" t="s">
         <v>205</v>
       </c>
@@ -41477,7 +41534,7 @@
       </c>
     </row>
     <row r="26" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B26" s="95"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="49" t="s">
         <v>206</v>
       </c>
@@ -41544,7 +41601,7 @@
       </c>
     </row>
     <row r="27" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B27" s="95"/>
+      <c r="B27" s="102"/>
       <c r="C27" s="49" t="s">
         <v>207</v>
       </c>
@@ -41611,7 +41668,7 @@
       </c>
     </row>
     <row r="28" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B28" s="102" t="s">
+      <c r="B28" s="109" t="s">
         <v>209</v>
       </c>
       <c r="C28" s="49" t="s">
@@ -41677,7 +41734,7 @@
       </c>
     </row>
     <row r="29" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B29" s="95"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="49" t="s">
         <v>205</v>
       </c>
@@ -41741,7 +41798,7 @@
       </c>
     </row>
     <row r="30" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B30" s="95"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="49" t="s">
         <v>206</v>
       </c>
@@ -41805,7 +41862,7 @@
       </c>
     </row>
     <row r="31" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B31" s="95"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="49" t="s">
         <v>207</v>
       </c>
@@ -54703,12 +54760,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="111" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
     </row>
     <row r="2" spans="1:12" ht="13">
       <c r="A2" s="57" t="s">
@@ -54810,12 +54867,12 @@
       <c r="D7" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="F7" s="98" t="s">
+      <c r="F7" s="105" t="s">
         <v>230</v>
       </c>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="F8" s="6" t="s">
@@ -55264,12 +55321,12 @@
     <row r="1" spans="1:19" ht="13">
       <c r="C1" s="66"/>
       <c r="H1" s="23"/>
-      <c r="I1" s="105" t="s">
+      <c r="I1" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="91"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="91"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="98"/>
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
@@ -70850,7 +70907,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -72537,8 +72594,8 @@
   <sheetPr codeName="Arkusz9"/>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -72550,15 +72607,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="114" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="D1" s="108" t="s">
+      <c r="B1" s="114"/>
+      <c r="D1" s="115" t="s">
         <v>295</v>
       </c>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
@@ -72633,13 +72690,13 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="13">
-      <c r="D6" s="108" t="s">
+      <c r="D6" s="115" t="s">
         <v>315</v>
       </c>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
     </row>
     <row r="7" spans="1:8">
       <c r="C7" s="80"/>
@@ -72679,11 +72736,11 @@
       </c>
       <c r="G8" s="87">
         <f xml:space="preserve"> E8/(F8*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-0.10396623227262985</v>
+        <v>-0.10446517388067798</v>
       </c>
       <c r="H8" s="87">
         <f xml:space="preserve"> DEGREES(G8)</f>
-        <v>-5.9568263210985037</v>
+        <v>-5.9854135694631321</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -72704,11 +72761,11 @@
       </c>
       <c r="G9" s="87">
         <f xml:space="preserve"> E9/(F9*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-7.2615299398383903E-2</v>
+        <v>-7.3114241006432046E-2</v>
       </c>
       <c r="H9" s="87">
         <f xml:space="preserve"> DEGREES(G9)</f>
-        <v>-4.1605501836062633</v>
+        <v>-4.1891374319708925</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -72730,11 +72787,11 @@
       </c>
       <c r="G10" s="87">
         <f xml:space="preserve"> E10/(F10*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-3.7987792448418198E-2</v>
+        <v>-3.8486734056466333E-2</v>
       </c>
       <c r="H10" s="87">
         <f t="shared" ref="H10" si="0" xml:space="preserve"> DEGREES(G10)</f>
-        <v>-2.1765401803133027</v>
+        <v>-2.2051274286779314</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -72769,6 +72826,9 @@
       <c r="C13" t="s">
         <v>319</v>
       </c>
+      <c r="G13" s="80" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -72802,7 +72862,7 @@
       <c r="A17" s="80" t="s">
         <v>338</v>
       </c>
-      <c r="B17" s="111">
+      <c r="B17" s="90">
         <f>3.1*52.11/100</f>
         <v>1.61541</v>
       </c>
@@ -72860,17 +72920,17 @@
       <c r="A25" s="80" t="s">
         <v>309</v>
       </c>
-      <c r="B25" s="112">
+      <c r="B25" s="91">
         <f>proj2_copy!H9</f>
         <v>6.5967841001666665</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="110" t="s">
+      <c r="F25" s="116" t="s">
         <v>328</v>
       </c>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="116"/>
+      <c r="I25" s="116"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
@@ -72886,14 +72946,14 @@
       <c r="F26" s="87" t="s">
         <v>320</v>
       </c>
-      <c r="G26" s="109">
+      <c r="G26" s="89">
         <f>B15</f>
         <v>0.45238095238095233</v>
       </c>
       <c r="H26" s="87" t="s">
         <v>326</v>
       </c>
-      <c r="I26" s="109">
+      <c r="I26" s="89">
         <f>B16</f>
         <v>0.15633</v>
       </c>
@@ -72910,7 +72970,7 @@
       <c r="F27" s="87" t="s">
         <v>321</v>
       </c>
-      <c r="G27" s="109">
+      <c r="G27" s="89">
         <f>B12</f>
         <v>0.80266666666666664</v>
       </c>
@@ -73047,12 +73107,18 @@
       </c>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="84">
-        <f xml:space="preserve"> 2*726*9.81/(1.225*15*54.4^2)</f>
-        <v>0.2619452192641763</v>
+      <c r="A36" s="92" t="s">
+        <v>349</v>
+      </c>
+      <c r="B36" s="93">
+        <f xml:space="preserve"> 2*726*9.81/(1.225*15*D36^2)</f>
+        <v>0.26584026203073824</v>
+      </c>
+      <c r="C36" s="95" t="s">
+        <v>350</v>
+      </c>
+      <c r="D36" s="94">
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -73087,10 +73153,10 @@
       </c>
       <c r="B39" s="84">
         <f>C39*E42</f>
-        <v>-1.4323944878270582</v>
+        <v>-0.2291831180523293</v>
       </c>
       <c r="C39">
-        <v>-2.5000000000000001E-2</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="F39" s="80" t="s">
         <v>337</v>
@@ -73106,7 +73172,7 @@
       </c>
       <c r="B40" s="84">
         <f xml:space="preserve"> B39*B33/B34</f>
-        <v>-0.90620875760487352</v>
+        <v>-0.14499340121677975</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -73150,7 +73216,7 @@
       </c>
       <c r="B45" s="84">
         <f xml:space="preserve"> B44+(B33/B34-1)*B40*B43</f>
-        <v>-0.15435210959222351</v>
+        <v>-0.32213018814306871</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -73171,7 +73237,7 @@
       </c>
       <c r="B48" s="84">
         <f xml:space="preserve"> B47*B20-(B33/B34-1)*B40*B42</f>
-        <v>-0.5690273780352233</v>
+        <v>-0.43760121650372785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pr9.v1:Fixed tables and final corections
</commit_message>
<xml_diff>
--- a/database/ml_projekty.xlsx
+++ b/database/ml_projekty.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\repos\MECHANIKA_LOTU\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECABE79-EF8E-40B6-8018-BAE08A6BCEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7451320C-941C-47DF-978E-F6C1721B06AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54795" yWindow="0" windowWidth="20085" windowHeight="15600" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46080" yWindow="0" windowWidth="8715" windowHeight="15600" xr2:uid="{216D74E0-F99A-467B-B9EA-B68CB369CAC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Baza" sheetId="10" r:id="rId1"/>
@@ -120,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="387">
   <si>
     <t>Co liczę</t>
   </si>
@@ -1292,6 +1293,12 @@
   <si>
     <t>Projekt 10</t>
   </si>
+  <si>
+    <t>deltaHk_rad</t>
+  </si>
+  <si>
+    <t>deltaHk_deg</t>
+  </si>
 </sst>
 </file>
 
@@ -1738,7 +1745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1959,6 +1966,7 @@
     <xf numFmtId="0" fontId="28" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2371,7 +2379,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>387768</xdr:colOff>
+      <xdr:colOff>390943</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>55254</xdr:rowOff>
     </xdr:to>
@@ -2415,9 +2423,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>145614</xdr:colOff>
+      <xdr:colOff>142439</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>102900</xdr:rowOff>
+      <xdr:rowOff>106075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2459,7 +2467,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>219617</xdr:colOff>
+      <xdr:colOff>216442</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>189099</xdr:rowOff>
     </xdr:to>
@@ -2503,9 +2511,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>292893</xdr:colOff>
+      <xdr:colOff>296068</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>141512</xdr:rowOff>
+      <xdr:rowOff>144687</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2547,9 +2555,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>277976</xdr:colOff>
+      <xdr:colOff>274801</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>64414</xdr:rowOff>
+      <xdr:rowOff>67589</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2591,9 +2599,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>276609</xdr:colOff>
+      <xdr:colOff>273434</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>104877</xdr:rowOff>
+      <xdr:rowOff>101702</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2841,10 +2849,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB95FAE-322E-4227-B7D5-16D9D30D119F}">
   <sheetPr codeName="Arkusz3"/>
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="H23" workbookViewId="1">
+      <selection activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -3317,7 +3328,8 @@
         <v>376</v>
       </c>
       <c r="N40">
-        <v>-0.10446517399999999</v>
+        <f xml:space="preserve"> 'Pr9'!G8</f>
+        <v>-0.16442302973386907</v>
       </c>
     </row>
     <row r="41" spans="13:14">
@@ -3325,7 +3337,8 @@
         <v>377</v>
       </c>
       <c r="N41">
-        <v>-7.3114240999999996E-2</v>
+        <f xml:space="preserve"> 'Pr9'!G9</f>
+        <v>-0.13307209685962312</v>
       </c>
     </row>
     <row r="42" spans="13:14">
@@ -3333,7 +3346,8 @@
         <v>378</v>
       </c>
       <c r="N42">
-        <v>-3.8486734000000002E-2</v>
+        <f xml:space="preserve"> 'Pr9'!G10</f>
+        <v>-9.8444589909657404E-2</v>
       </c>
     </row>
     <row r="45" spans="13:14">
@@ -3438,6 +3452,23 @@
       </c>
       <c r="N61">
         <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="13:14">
+      <c r="M63" t="s">
+        <v>385</v>
+      </c>
+      <c r="N63" s="126">
+        <f xml:space="preserve"> 0.0334</f>
+        <v>3.3399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="13:14">
+      <c r="M64" t="s">
+        <v>386</v>
+      </c>
+      <c r="N64">
+        <v>1.913</v>
       </c>
     </row>
   </sheetData>
@@ -3464,6 +3495,7 @@
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -37702,6 +37734,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -40105,6 +40138,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30:B30"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -40919,6 +40953,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -55503,6 +55538,9 @@
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -56067,6 +56105,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -71664,9 +71703,10 @@
   <sheetPr codeName="Arkusz8"/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
@@ -73352,8 +73392,11 @@
   <sheetPr codeName="Arkusz9"/>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -73494,11 +73537,11 @@
       </c>
       <c r="G8" s="87">
         <f xml:space="preserve"> E8/(F8*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-0.10446517388067798</v>
+        <v>-0.16442302973386907</v>
       </c>
       <c r="H8" s="87">
         <f xml:space="preserve"> DEGREES(G8)</f>
-        <v>-5.9854135694631321</v>
+        <v>-9.4207456585047407</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -73519,11 +73562,11 @@
       </c>
       <c r="G9" s="87">
         <f xml:space="preserve"> E9/(F9*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-7.3114241006432046E-2</v>
+        <v>-0.13307209685962312</v>
       </c>
       <c r="H9" s="87">
         <f xml:space="preserve"> DEGREES(G9)</f>
-        <v>-4.1891374319708925</v>
+        <v>-7.6244695210125011</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -73545,11 +73588,11 @@
       </c>
       <c r="G10" s="87">
         <f xml:space="preserve"> E10/(F10*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-3.8486734056466333E-2</v>
+        <v>-9.8444589909657404E-2</v>
       </c>
       <c r="H10" s="87">
         <f t="shared" ref="H10" si="0" xml:space="preserve"> DEGREES(G10)</f>
-        <v>-2.2051274286779314</v>
+        <v>-5.6404595177195391</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -73870,13 +73913,13 @@
       </c>
       <c r="B36" s="93">
         <f xml:space="preserve"> 2*726*9.81/(1.225*15*D36^2)</f>
-        <v>0.26584026203073824</v>
+        <v>0.73390788552107233</v>
       </c>
       <c r="C36" s="95" t="s">
         <v>349</v>
       </c>
       <c r="D36" s="94">
-        <v>54</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="37" spans="1:17">

</xml_diff>

<commit_message>
proj10:skonczony ale jeszcze nie zweryfikowany czy poprawny
</commit_message>
<xml_diff>
--- a/database/ml_projekty.xlsx
+++ b/database/ml_projekty.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\repos\MECHANIKA_LOTU\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7451320C-941C-47DF-978E-F6C1721B06AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630083C7-02E5-49F9-9699-96DA76C285F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54795" yWindow="0" windowWidth="20085" windowHeight="15600" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="46080" yWindow="0" windowWidth="8715" windowHeight="15600" xr2:uid="{216D74E0-F99A-467B-B9EA-B68CB369CAC9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="18600" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="310" yWindow="270" windowWidth="7500" windowHeight="6000" firstSheet="3" activeTab="9" xr2:uid="{F3B987AC-2077-4658-9C8D-A231F3196A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Baza" sheetId="10" r:id="rId1"/>
@@ -23,11 +23,13 @@
     <sheet name="proj8" sheetId="6" r:id="rId7"/>
     <sheet name="Base_pr8" sheetId="9" r:id="rId8"/>
     <sheet name="Pr9" sheetId="8" r:id="rId9"/>
+    <sheet name="proj10" sheetId="11" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -121,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="405">
   <si>
     <t>Co liczę</t>
   </si>
@@ -1299,6 +1301,60 @@
   <si>
     <t>deltaHk_deg</t>
   </si>
+  <si>
+    <t>pdh</t>
+  </si>
+  <si>
+    <t>kghn</t>
+  </si>
+  <si>
+    <t>kghn'</t>
+  </si>
+  <si>
+    <t>kghm</t>
+  </si>
+  <si>
+    <t>kghm'</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>kappa'_h</t>
+  </si>
+  <si>
+    <t>bar_xsa</t>
+  </si>
+  <si>
+    <t>bar_zs</t>
+  </si>
+  <si>
+    <t>delta_xsak</t>
+  </si>
+  <si>
+    <t>xsaj</t>
+  </si>
+  <si>
+    <t>xsah</t>
+  </si>
+  <si>
+    <t>alpha_0</t>
+  </si>
+  <si>
+    <t>m_calc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho </t>
+  </si>
+  <si>
+    <t>kdh</t>
+  </si>
+  <si>
+    <t>x_sah</t>
+  </si>
+  <si>
+    <t>ldH</t>
+  </si>
 </sst>
 </file>
 
@@ -1310,7 +1366,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1520,6 +1576,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
       <charset val="238"/>
     </font>
   </fonts>
@@ -1745,7 +1808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1903,6 +1966,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1966,7 +2031,6 @@
     <xf numFmtId="0" fontId="28" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2062,9 +2126,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3819525" cy="647700"/>
     <xdr:pic>
@@ -2086,7 +2150,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2778125" y="901700"/>
+          <a:off x="2844800" y="679450"/>
           <a:ext cx="3819525" cy="647700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2100,9 +2164,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3657600" cy="533400"/>
     <xdr:pic>
@@ -2124,7 +2188,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2682875" y="2028825"/>
+          <a:off x="2292350" y="3451225"/>
           <a:ext cx="3657600" cy="533400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2849,43 +2913,43 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB95FAE-322E-4227-B7D5-16D9D30D119F}">
   <sheetPr codeName="Arkusz3"/>
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="H23" workbookViewId="1">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
     <row r="1" spans="1:17" s="98" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>381</v>
       </c>
-      <c r="B1" s="103"/>
+      <c r="B1" s="105"/>
       <c r="C1" s="99"/>
-      <c r="D1" s="104" t="s">
+      <c r="D1" s="106" t="s">
         <v>356</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="G1" s="101" t="s">
+      <c r="E1" s="106"/>
+      <c r="G1" s="103" t="s">
         <v>357</v>
       </c>
-      <c r="H1" s="101"/>
-      <c r="J1" s="101" t="s">
+      <c r="H1" s="103"/>
+      <c r="J1" s="103" t="s">
         <v>362</v>
       </c>
-      <c r="K1" s="101"/>
-      <c r="M1" s="101" t="s">
+      <c r="K1" s="103"/>
+      <c r="M1" s="103" t="s">
         <v>366</v>
       </c>
-      <c r="N1" s="101"/>
-      <c r="P1" s="101" t="s">
+      <c r="N1" s="103"/>
+      <c r="P1" s="103" t="s">
         <v>384</v>
       </c>
-      <c r="Q1" s="101"/>
+      <c r="Q1" s="103"/>
     </row>
     <row r="2" spans="1:17" s="97" customFormat="1" ht="13.5" customHeight="1">
       <c r="A2" s="100" t="s">
@@ -2934,10 +2998,10 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>309</v>
+        <v>62</v>
       </c>
       <c r="E3">
-        <v>6.59</v>
+        <v>4.452</v>
       </c>
       <c r="G3" t="s">
         <v>358</v>
@@ -2957,7 +3021,12 @@
       <c r="N3">
         <v>2.86</v>
       </c>
-      <c r="P3" s="80"/>
+      <c r="P3" s="80" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q3">
+        <v>0.95279999999999998</v>
+      </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -2966,12 +3035,6 @@
       <c r="B4">
         <v>9.94</v>
       </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4">
-        <v>4.452</v>
-      </c>
       <c r="G4" t="s">
         <v>359</v>
       </c>
@@ -2983,6 +3046,19 @@
       </c>
       <c r="K4">
         <v>0.25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>403</v>
+      </c>
+      <c r="N4">
+        <f xml:space="preserve"> N3*1.5</f>
+        <v>4.29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q4">
+        <v>0.97609999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -3004,11 +3080,11 @@
       <c r="K5">
         <v>0.38</v>
       </c>
-      <c r="M5" t="s">
-        <v>368</v>
-      </c>
-      <c r="N5">
-        <v>0.34</v>
+      <c r="P5" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q5">
+        <v>0.94779999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -3025,10 +3101,16 @@
         <v>3.01</v>
       </c>
       <c r="M6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N6">
-        <v>0.33</v>
+        <v>0.34</v>
+      </c>
+      <c r="P6" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q6">
+        <v>0.96360000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -3044,11 +3126,23 @@
       <c r="H7">
         <v>2.2000000000000002</v>
       </c>
+      <c r="J7" s="80" t="s">
+        <v>399</v>
+      </c>
+      <c r="K7">
+        <v>-2.5</v>
+      </c>
       <c r="M7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N7">
-        <v>0.31</v>
+        <v>0.33</v>
+      </c>
+      <c r="P7" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q7">
+        <v>16.45</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -3064,6 +3158,18 @@
       <c r="H8">
         <v>5.09</v>
       </c>
+      <c r="M8" t="s">
+        <v>370</v>
+      </c>
+      <c r="N8">
+        <v>0.31</v>
+      </c>
+      <c r="P8" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q8">
+        <v>0.35730000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
@@ -3078,12 +3184,7 @@
       <c r="H9">
         <v>-4.8000000000000001E-2</v>
       </c>
-      <c r="M9" t="s">
-        <v>299</v>
-      </c>
-      <c r="N9">
-        <v>3.01</v>
-      </c>
+      <c r="J9" s="80"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
@@ -3099,10 +3200,16 @@
         <v>0.42299999999999999</v>
       </c>
       <c r="M10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N10">
-        <v>2.2000000000000002</v>
+        <v>3.01</v>
+      </c>
+      <c r="P10" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q10">
+        <v>0.24</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -3119,10 +3226,16 @@
         <v>-2.3999999999999998E-3</v>
       </c>
       <c r="M11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N11">
-        <v>0.73</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q11" s="66">
+        <v>-0.23699999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -3133,342 +3246,397 @@
         <v>0.85</v>
       </c>
       <c r="M12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N12">
-        <v>1.0940000000000001</v>
+        <v>0.73</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q12" s="66">
+        <v>-2.52E-2</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="M13" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="N13">
-        <v>0.80300000000000005</v>
+        <v>1.0940000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="M14" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="N14">
-        <v>0.26100000000000001</v>
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="P14" s="80" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q14" s="66">
+        <v>-2.52E-2</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="M15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N15">
-        <v>0.46899999999999997</v>
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="P15" s="80" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q15" s="66">
+        <v>0.03</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="M16" t="s">
+        <v>324</v>
+      </c>
+      <c r="N16">
+        <v>0.46899999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="13:19">
+      <c r="M17" t="s">
         <v>322</v>
       </c>
-      <c r="N16">
+      <c r="N17">
         <v>0.45200000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="13:14">
-      <c r="M17" t="s">
+      <c r="P17" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q17" s="66">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="18" spans="13:19">
+      <c r="M18" t="s">
         <v>340</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>0.156</v>
       </c>
-    </row>
-    <row r="18" spans="13:14">
-      <c r="M18" t="s">
+      <c r="P18" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q18" s="66">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="13:19">
+      <c r="M19" t="s">
         <v>338</v>
       </c>
-      <c r="N18">
+      <c r="N19">
         <v>1.615</v>
       </c>
     </row>
-    <row r="19" spans="13:14">
-      <c r="M19" t="s">
+    <row r="20" spans="13:19">
+      <c r="M20" t="s">
         <v>339</v>
       </c>
-      <c r="N19">
+      <c r="N20">
         <v>0.253</v>
       </c>
-    </row>
-    <row r="20" spans="13:14">
-      <c r="M20" t="s">
+      <c r="P20" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q20" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="13:19">
+      <c r="M21" t="s">
         <v>341</v>
       </c>
-      <c r="N20">
+      <c r="N21">
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="21" spans="13:14">
-      <c r="M21" t="s">
+    <row r="22" spans="13:19">
+      <c r="M22" t="s">
         <v>337</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="13:14">
-      <c r="M23" t="s">
+    <row r="24" spans="13:19">
+      <c r="M24" t="s">
         <v>301</v>
       </c>
-      <c r="N23">
+      <c r="N24">
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="13:14">
-      <c r="M24" t="s">
+    <row r="25" spans="13:19">
+      <c r="M25" t="s">
         <v>304</v>
       </c>
-      <c r="N24">
+      <c r="N25">
         <v>4.1180000000000003</v>
       </c>
     </row>
-    <row r="26" spans="13:14">
-      <c r="M26" t="s">
-        <v>309</v>
-      </c>
-      <c r="N26">
-        <v>6.5970000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="13:14">
-      <c r="M27" t="s">
+    <row r="28" spans="13:19">
+      <c r="M28" t="s">
         <v>371</v>
       </c>
-      <c r="N27">
+      <c r="N28">
         <v>0.93400000000000005</v>
       </c>
-    </row>
-    <row r="28" spans="13:14">
-      <c r="M28" t="s">
+      <c r="S28" s="102" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="29" spans="13:19">
+      <c r="M29" t="s">
         <v>342</v>
       </c>
-      <c r="N28">
+      <c r="N29">
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="29" spans="13:14">
-      <c r="M29" t="s">
+    <row r="30" spans="13:19">
+      <c r="M30" t="s">
         <v>343</v>
       </c>
-      <c r="N29">
+      <c r="N30">
         <v>0.27</v>
       </c>
     </row>
-    <row r="31" spans="13:14">
-      <c r="M31" t="s">
+    <row r="32" spans="13:19">
+      <c r="M32" t="s">
         <v>372</v>
       </c>
-      <c r="N31">
+      <c r="N32">
         <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="13:14">
-      <c r="M32" t="s">
-        <v>331</v>
-      </c>
-      <c r="N32">
-        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="33" spans="13:14">
       <c r="M33" t="s">
-        <v>305</v>
+        <v>331</v>
       </c>
       <c r="N33">
-        <v>3.1</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="34" spans="13:14">
       <c r="M34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N34">
-        <v>2.218</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="35" spans="13:14">
       <c r="M35" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="N35">
-        <v>0.43</v>
+        <v>2.218</v>
       </c>
     </row>
     <row r="36" spans="13:14">
       <c r="M36" t="s">
-        <v>373</v>
+        <v>308</v>
       </c>
       <c r="N36">
-        <v>0.34</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="37" spans="13:14">
       <c r="M37" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N37">
-        <v>0.326344089</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="38" spans="13:14">
       <c r="M38" t="s">
+        <v>374</v>
+      </c>
+      <c r="N38">
+        <v>0.326344089</v>
+      </c>
+    </row>
+    <row r="39" spans="13:14">
+      <c r="M39" t="s">
         <v>375</v>
       </c>
-      <c r="N38">
+      <c r="N39">
         <v>0.310137422</v>
       </c>
     </row>
-    <row r="40" spans="13:14">
-      <c r="M40" t="s">
+    <row r="41" spans="13:14">
+      <c r="M41" t="s">
         <v>376</v>
       </c>
-      <c r="N40">
+      <c r="N41">
         <f xml:space="preserve"> 'Pr9'!G8</f>
         <v>-0.16442302973386907</v>
       </c>
     </row>
-    <row r="41" spans="13:14">
-      <c r="M41" t="s">
+    <row r="42" spans="13:14">
+      <c r="M42" t="s">
         <v>377</v>
       </c>
-      <c r="N41">
+      <c r="N42">
         <f xml:space="preserve"> 'Pr9'!G9</f>
         <v>-0.13307209685962312</v>
       </c>
     </row>
-    <row r="42" spans="13:14">
-      <c r="M42" t="s">
+    <row r="43" spans="13:14">
+      <c r="M43" t="s">
         <v>378</v>
       </c>
-      <c r="N42">
+      <c r="N43">
         <f xml:space="preserve"> 'Pr9'!G10</f>
         <v>-9.8444589909657404E-2</v>
       </c>
     </row>
-    <row r="45" spans="13:14">
-      <c r="M45" t="s">
-        <v>261</v>
-      </c>
-      <c r="N45">
-        <v>-7.4770964999999995E-2</v>
-      </c>
-    </row>
     <row r="46" spans="13:14">
       <c r="M46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N46">
-        <v>-3.9516728000000001E-2</v>
+        <v>-7.4770964999999995E-2</v>
       </c>
     </row>
     <row r="47" spans="13:14">
       <c r="M47" t="s">
+        <v>262</v>
+      </c>
+      <c r="N47">
+        <v>-3.9516728000000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="13:14">
+      <c r="M48" t="s">
         <v>263</v>
       </c>
-      <c r="N47">
+      <c r="N48">
         <v>-4.2624910000000002E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="13:14">
-      <c r="M49" t="s">
-        <v>379</v>
-      </c>
-      <c r="N49">
-        <v>0</v>
       </c>
     </row>
     <row r="50" spans="13:14">
       <c r="M50" t="s">
-        <v>333</v>
+        <v>379</v>
       </c>
       <c r="N50">
-        <v>-0.22900000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="13:14">
       <c r="M51" t="s">
+        <v>333</v>
+      </c>
+      <c r="N51">
+        <v>-0.22900000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="13:14">
+      <c r="M52" t="s">
         <v>332</v>
       </c>
-      <c r="N51">
+      <c r="N52">
         <v>-0.14499999999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="13:14">
-      <c r="M53" t="s">
-        <v>350</v>
-      </c>
-      <c r="N53">
-        <v>0.47</v>
       </c>
     </row>
     <row r="54" spans="13:14">
       <c r="M54" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="N54">
-        <v>0.6</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="55" spans="13:14">
       <c r="M55" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="N55">
-        <v>-0.35399999999999998</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="56" spans="13:14">
       <c r="M56" t="s">
+        <v>334</v>
+      </c>
+      <c r="N56">
+        <v>-0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="13:14">
+      <c r="M57" t="s">
         <v>335</v>
       </c>
-      <c r="N56">
+      <c r="N57">
         <v>-0.32200000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="13:14">
-      <c r="M58" t="s">
-        <v>346</v>
-      </c>
-      <c r="N58">
-        <v>-1.4319999999999999</v>
       </c>
     </row>
     <row r="59" spans="13:14">
       <c r="M59" t="s">
+        <v>346</v>
+      </c>
+      <c r="N59">
+        <v>-1.4319999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="13:14">
+      <c r="M60" t="s">
         <v>344</v>
       </c>
-      <c r="N59">
+      <c r="N60">
         <v>-0.38800000000000001</v>
       </c>
     </row>
-    <row r="61" spans="13:14">
-      <c r="M61" t="s">
+    <row r="62" spans="13:14">
+      <c r="M62" t="s">
         <v>380</v>
       </c>
-      <c r="N61">
+      <c r="N62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="13:14">
-      <c r="M63" t="s">
+    <row r="64" spans="13:14">
+      <c r="M64" t="s">
         <v>385</v>
       </c>
-      <c r="N63" s="126">
+      <c r="N64" s="101">
         <f xml:space="preserve"> 0.0334</f>
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="64" spans="13:14">
-      <c r="M64" t="s">
+    <row r="65" spans="13:14">
+      <c r="M65" t="s">
         <v>386</v>
       </c>
-      <c r="N64">
+      <c r="N65">
         <v>1.913</v>
+      </c>
+    </row>
+    <row r="67" spans="13:14">
+      <c r="M67" s="80" t="s">
+        <v>387</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="13:14">
+      <c r="M69" t="s">
+        <v>404</v>
+      </c>
+      <c r="N69">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3481,7 +3649,20 @@
     <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0630668A-DD81-4993-A908-00B1F0E99DB2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -37734,7 +37915,9 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="E18" sqref="E18:E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -37744,35 +37927,35 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="23"/>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="105" t="s">
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="105" t="s">
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="107" t="s">
         <v>166</v>
       </c>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="108" t="s">
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="110" t="s">
         <v>167</v>
       </c>
-      <c r="S1" s="109"/>
-      <c r="T1" s="109"/>
-      <c r="U1" s="109"/>
-      <c r="V1" s="109"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="39" t="s">
@@ -40284,7 +40467,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="13">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="114" t="s">
         <v>86</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -40302,7 +40485,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A9" s="111"/>
+      <c r="A9" s="113"/>
       <c r="B9" s="6" t="s">
         <v>89</v>
       </c>
@@ -40323,7 +40506,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A10" s="111"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="21" t="s">
         <v>92</v>
       </c>
@@ -40341,7 +40524,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A11" s="111"/>
+      <c r="A11" s="113"/>
       <c r="B11" s="21" t="s">
         <v>95</v>
       </c>
@@ -40392,14 +40575,14 @@
       <c r="B18" s="6">
         <v>1.5</v>
       </c>
-      <c r="E18" s="113" t="s">
+      <c r="E18" s="115" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="106"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="107"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="109"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="6" t="s">
@@ -40676,10 +40859,10 @@
         <f>0.355/B18</f>
         <v>0.23666666666666666</v>
       </c>
-      <c r="E32" s="114" t="s">
+      <c r="E32" s="116" t="s">
         <v>134</v>
       </c>
-      <c r="F32" s="111"/>
+      <c r="F32" s="113"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="21" t="s">
@@ -40729,10 +40912,10 @@
         <f>1/B35*(B27+B33*(B31-B32))</f>
         <v>-0.10312152368291011</v>
       </c>
-      <c r="E37" s="115" t="s">
+      <c r="E37" s="117" t="s">
         <v>141</v>
       </c>
-      <c r="F37" s="111"/>
+      <c r="F37" s="113"/>
     </row>
     <row r="38" spans="1:6" ht="15.5">
       <c r="E38" s="6" t="s">
@@ -40791,10 +40974,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="13">
-      <c r="A48" s="110" t="s">
+      <c r="A48" s="112" t="s">
         <v>149</v>
       </c>
-      <c r="B48" s="111"/>
+      <c r="B48" s="113"/>
     </row>
     <row r="49" spans="1:3" ht="12.5">
       <c r="A49" s="6" t="s">
@@ -40841,10 +41024,10 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="13">
-      <c r="A55" s="110" t="s">
+      <c r="A55" s="112" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="111"/>
+      <c r="B55" s="113"/>
     </row>
     <row r="56" spans="1:3" ht="12.5">
       <c r="A56" s="6" t="s">
@@ -40856,10 +41039,10 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="13">
-      <c r="A58" s="110" t="s">
+      <c r="A58" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="B58" s="111"/>
+      <c r="B58" s="113"/>
     </row>
     <row r="59" spans="1:3" ht="12.5">
       <c r="A59" s="6" t="s">
@@ -40969,33 +41152,33 @@
       <c r="B1" s="6">
         <v>600</v>
       </c>
-      <c r="I1" s="119" t="s">
+      <c r="I1" s="121" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="119" t="s">
+      <c r="J1" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="119" t="s">
+      <c r="K1" s="121" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="119" t="s">
+      <c r="L1" s="121" t="s">
         <v>173</v>
       </c>
-      <c r="M1" s="119" t="s">
+      <c r="M1" s="121" t="s">
         <v>170</v>
       </c>
-      <c r="N1" s="116" t="s">
+      <c r="N1" s="118" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="111"/>
-      <c r="P1" s="117" t="s">
+      <c r="O1" s="113"/>
+      <c r="P1" s="119" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="117" t="s">
+      <c r="Q1" s="113"/>
+      <c r="R1" s="119" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="111"/>
+      <c r="S1" s="113"/>
     </row>
     <row r="2" spans="1:19" ht="13">
       <c r="A2" s="21" t="s">
@@ -41004,11 +41187,11 @@
       <c r="B2" s="6">
         <v>726</v>
       </c>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
       <c r="N2" s="41" t="s">
         <v>178</v>
       </c>
@@ -41329,15 +41512,15 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="13">
-      <c r="A9" s="110" t="s">
+      <c r="A9" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="111"/>
-      <c r="D9" s="110" t="s">
+      <c r="B9" s="113"/>
+      <c r="D9" s="112" t="s">
         <v>190</v>
       </c>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
       <c r="I9" s="42">
         <v>1.5</v>
       </c>
@@ -41926,7 +42109,7 @@
       </c>
     </row>
     <row r="20" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B20" s="118" t="s">
+      <c r="B20" s="120" t="s">
         <v>203</v>
       </c>
       <c r="C20" s="49" t="s">
@@ -41992,7 +42175,7 @@
       </c>
     </row>
     <row r="21" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B21" s="111"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="49" t="s">
         <v>205</v>
       </c>
@@ -42056,7 +42239,7 @@
       </c>
     </row>
     <row r="22" spans="2:21" ht="13">
-      <c r="B22" s="111"/>
+      <c r="B22" s="113"/>
       <c r="C22" s="49" t="s">
         <v>206</v>
       </c>
@@ -42124,7 +42307,7 @@
       </c>
     </row>
     <row r="23" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B23" s="111"/>
+      <c r="B23" s="113"/>
       <c r="C23" s="49" t="s">
         <v>207</v>
       </c>
@@ -42191,7 +42374,7 @@
       </c>
     </row>
     <row r="24" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B24" s="118" t="s">
+      <c r="B24" s="120" t="s">
         <v>208</v>
       </c>
       <c r="C24" s="49" t="s">
@@ -42260,7 +42443,7 @@
       </c>
     </row>
     <row r="25" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B25" s="111"/>
+      <c r="B25" s="113"/>
       <c r="C25" s="49" t="s">
         <v>205</v>
       </c>
@@ -42327,7 +42510,7 @@
       </c>
     </row>
     <row r="26" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B26" s="111"/>
+      <c r="B26" s="113"/>
       <c r="C26" s="49" t="s">
         <v>206</v>
       </c>
@@ -42394,7 +42577,7 @@
       </c>
     </row>
     <row r="27" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B27" s="111"/>
+      <c r="B27" s="113"/>
       <c r="C27" s="49" t="s">
         <v>207</v>
       </c>
@@ -42461,7 +42644,7 @@
       </c>
     </row>
     <row r="28" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B28" s="118" t="s">
+      <c r="B28" s="120" t="s">
         <v>209</v>
       </c>
       <c r="C28" s="49" t="s">
@@ -42527,7 +42710,7 @@
       </c>
     </row>
     <row r="29" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B29" s="111"/>
+      <c r="B29" s="113"/>
       <c r="C29" s="49" t="s">
         <v>205</v>
       </c>
@@ -42591,7 +42774,7 @@
       </c>
     </row>
     <row r="30" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B30" s="111"/>
+      <c r="B30" s="113"/>
       <c r="C30" s="49" t="s">
         <v>206</v>
       </c>
@@ -42655,7 +42838,7 @@
       </c>
     </row>
     <row r="31" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B31" s="111"/>
+      <c r="B31" s="113"/>
       <c r="C31" s="49" t="s">
         <v>207</v>
       </c>
@@ -55556,12 +55739,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
     </row>
     <row r="2" spans="1:12" ht="13">
       <c r="A2" s="57" t="s">
@@ -55663,12 +55846,12 @@
       <c r="D7" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="116" t="s">
         <v>230</v>
       </c>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="113"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="F8" s="6" t="s">
@@ -56105,7 +56288,9 @@
     <sheetView workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A4" workbookViewId="1">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -56118,12 +56303,12 @@
     <row r="1" spans="1:19" ht="13">
       <c r="C1" s="66"/>
       <c r="H1" s="23"/>
-      <c r="I1" s="121" t="s">
+      <c r="I1" s="123" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="107"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="107"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="109"/>
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
@@ -71703,7 +71888,7 @@
   <sheetPr codeName="Arkusz8"/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
@@ -73392,8 +73577,8 @@
   <sheetPr codeName="Arkusz9"/>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection sqref="A1:B1"/>
@@ -73408,15 +73593,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="125" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="D1" s="124" t="s">
+      <c r="B1" s="125"/>
+      <c r="D1" s="126" t="s">
         <v>295</v>
       </c>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
@@ -73491,13 +73676,13 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="13">
-      <c r="D6" s="124" t="s">
+      <c r="D6" s="126" t="s">
         <v>315</v>
       </c>
-      <c r="E6" s="124"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
     </row>
     <row r="7" spans="1:8">
       <c r="C7" s="80"/>
@@ -73726,12 +73911,12 @@
         <v>6.5967841001666665</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="125" t="s">
+      <c r="F25" s="127" t="s">
         <v>328</v>
       </c>
-      <c r="G25" s="125"/>
-      <c r="H25" s="125"/>
-      <c r="I25" s="125"/>
+      <c r="G25" s="127"/>
+      <c r="H25" s="127"/>
+      <c r="I25" s="127"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
mam nadzieje ze to  ostatni commit ugh
</commit_message>
<xml_diff>
--- a/database/ml_projekty.xlsx
+++ b/database/ml_projekty.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="Ten_skoroszyt"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\repos\MECHANIKA_LOTU\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630083C7-02E5-49F9-9699-96DA76C285F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DC21D4-2B76-485D-8667-D5022C1C42B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="18600" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView minimized="1" xWindow="310" yWindow="270" windowWidth="7500" windowHeight="6000" firstSheet="3" activeTab="9" xr2:uid="{F3B987AC-2077-4658-9C8D-A231F3196A13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="18820" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baza" sheetId="10" r:id="rId1"/>
@@ -29,7 +28,6 @@
     <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2915,11 +2913,8 @@
   <sheetPr codeName="Arkusz3"/>
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -3277,7 +3272,7 @@
         <v>398</v>
       </c>
       <c r="Q14" s="66">
-        <v>-2.52E-2</v>
+        <v>2.52E-2</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -3481,7 +3476,7 @@
       </c>
       <c r="N41">
         <f xml:space="preserve"> 'Pr9'!G8</f>
-        <v>-0.16442302973386907</v>
+        <v>-0.13398601185628983</v>
       </c>
     </row>
     <row r="42" spans="13:14">
@@ -3490,7 +3485,7 @@
       </c>
       <c r="N42">
         <f xml:space="preserve"> 'Pr9'!G9</f>
-        <v>-0.13307209685962312</v>
+        <v>-0.10263507898204391</v>
       </c>
     </row>
     <row r="43" spans="13:14">
@@ -3499,7 +3494,7 @@
       </c>
       <c r="N43">
         <f xml:space="preserve"> 'Pr9'!G10</f>
-        <v>-9.8444589909657404E-2</v>
+        <v>-6.800757203207819E-2</v>
       </c>
     </row>
     <row r="46" spans="13:14">
@@ -3655,10 +3650,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0630668A-DD81-4993-A908-00B1F0E99DB2}">
+  <sheetPr codeName="Arkusz10"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData/>
@@ -3673,15 +3668,16 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="17.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.90625" customWidth="1"/>
+    <col min="22" max="22" width="9" customWidth="1"/>
     <col min="26" max="26" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3751,7 +3747,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="5">
-        <v>1.6131</v>
+        <v>2.1</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -3828,7 +3824,7 @@
         <v>26</v>
       </c>
       <c r="H3" s="5">
-        <v>1.1291700000000002</v>
+        <v>1.6</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -3852,19 +3848,19 @@
       </c>
       <c r="Q3" s="7">
         <f t="shared" ref="Q3:Q45" si="1">N3+($H$19-$H$18)*(1-ABS(M3/$H$23))</f>
-        <v>1.1882728594935488E-2</v>
+        <v>1.1964947319872637E-2</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" ref="R3:R45" si="2">Q3 + $H$21 + M3^2/(PI() * $H$9) * (1+$H$33)</f>
-        <v>4.8312366259894768E-2</v>
+        <v>7.8104503661331551E-2</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" ref="S3:S45" si="3">M3/(PI() *$H$9) *(1+ $H$28) *180/PI()</f>
-        <v>-2.4022324632937222</v>
+        <v>-4.3872529064428099</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" ref="T3:T45" si="4">S3 +L3</f>
-        <v>-20.91651817757942</v>
+        <v>-22.901538620728509</v>
       </c>
       <c r="U3" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M3*(proj3!$B$31-proj3!$B$32))</f>
@@ -3880,7 +3876,7 @@
       </c>
       <c r="X3" s="7">
         <f>(R3+ W3+proj3!$B$25/proj3!$B$17 * V3)*(1+proj3!$F$33)</f>
-        <v>9.7975114724642806E-2</v>
+        <v>0.12985270174418018</v>
       </c>
       <c r="Y3" s="7">
         <f>M3 + U3 * proj3!$B$25/proj3!$B$17</f>
@@ -3888,11 +3884,11 @@
       </c>
       <c r="Z3" s="7">
         <f t="shared" ref="Z3:Z45" si="5">Y3/X3</f>
-        <v>-8.9499327437642844</v>
+        <v>-6.752810496585937</v>
       </c>
       <c r="AA3" s="7">
         <f t="shared" ref="AA3:AA45" si="6">Y3 ^3/X3^2</f>
-        <v>-70.238478584383685</v>
+        <v>-39.985697586592643</v>
       </c>
       <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
@@ -3916,7 +3912,7 @@
         <v>28</v>
       </c>
       <c r="H4" s="5">
-        <v>9.9474499999999999</v>
+        <v>17.8</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -3940,19 +3936,19 @@
       </c>
       <c r="Q4" s="7">
         <f t="shared" si="1"/>
-        <v>1.2733446744287063E-2</v>
+        <v>1.2811444854794829E-2</v>
       </c>
       <c r="R4" s="7">
         <f t="shared" si="2"/>
-        <v>5.2465879485296546E-2</v>
+        <v>8.5019431239360829E-2</v>
       </c>
       <c r="S4" s="7">
         <f t="shared" si="3"/>
-        <v>-2.5115543571477978</v>
+        <v>-4.5869100186822784</v>
       </c>
       <c r="T4" s="7">
         <f t="shared" si="4"/>
-        <v>-19.654411500004898</v>
+        <v>-21.729767161539378</v>
       </c>
       <c r="U4" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M4*(proj3!$B$31-proj3!$B$32))</f>
@@ -3968,7 +3964,7 @@
       </c>
       <c r="X4" s="7">
         <f>(R4+ W4+proj3!$B$25/proj3!$B$17 * V4)*(1+proj3!$F$33)</f>
-        <v>0.1027572022894528</v>
+        <v>0.13758950266630154</v>
       </c>
       <c r="Y4" s="7">
         <f>M4 + U4 * proj3!$B$25/proj3!$B$17</f>
@@ -3976,11 +3972,11 @@
       </c>
       <c r="Z4" s="7">
         <f t="shared" si="5"/>
-        <v>-8.9144031102874788</v>
+        <v>-6.657623626383594</v>
       </c>
       <c r="AA4" s="7">
         <f t="shared" si="6"/>
-        <v>-72.792909551012201</v>
+        <v>-40.601587990813357</v>
       </c>
       <c r="AB4" s="11"/>
       <c r="AC4" s="11"/>
@@ -4027,19 +4023,19 @@
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="1"/>
-        <v>1.4028358719184135E-2</v>
+        <v>1.4100383745896544E-2</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="2"/>
-        <v>5.868612261359088E-2</v>
+        <v>9.5357986245087289E-2</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" si="3"/>
-        <v>-2.666268521064636</v>
+        <v>-4.8694680873470189</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="4"/>
-        <v>-19.237697092493136</v>
+        <v>-21.440896658775518</v>
       </c>
       <c r="U5" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M5*(proj3!$B$31-proj3!$B$32))</f>
@@ -4055,7 +4051,7 @@
       </c>
       <c r="X5" s="7">
         <f>(R5+ W5+proj3!$B$25/proj3!$B$17 * V5)*(1+proj3!$F$33)</f>
-        <v>0.10989168049861914</v>
+        <v>0.14913057458432027</v>
       </c>
       <c r="Y5" s="7">
         <f>M5 + U5 * proj3!$B$25/proj3!$B$17</f>
@@ -4063,11 +4059,11 @@
       </c>
       <c r="Z5" s="7">
         <f t="shared" si="5"/>
-        <v>-8.8398197029402912</v>
+        <v>-6.5139066564224795</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="6"/>
-        <v>-75.909308722927278</v>
+        <v>-41.218414644432073</v>
       </c>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
@@ -4091,7 +4087,7 @@
         <v>31</v>
       </c>
       <c r="H6" s="5">
-        <v>15</v>
+        <v>27.8</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -4115,19 +4111,19 @@
       </c>
       <c r="Q6" s="7">
         <f t="shared" si="1"/>
-        <v>1.6272243510243027E-2</v>
+        <v>1.6338606304962266E-2</v>
       </c>
       <c r="R6" s="7">
         <f t="shared" si="2"/>
-        <v>6.5870774879238758E-2</v>
+        <v>0.10667418702817841</v>
       </c>
       <c r="S6" s="7">
         <f t="shared" si="3"/>
-        <v>-2.8129310355612804</v>
+        <v>-5.1373212417871104</v>
       </c>
       <c r="T6" s="7">
         <f t="shared" si="4"/>
-        <v>-18.927216749846981</v>
+        <v>-21.251606956072809</v>
       </c>
       <c r="U6" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M6*(proj3!$B$31-proj3!$B$32))</f>
@@ -4143,7 +4139,7 @@
       </c>
       <c r="X6" s="7">
         <f>(R6+ W6+proj3!$B$25/proj3!$B$17 * V6)*(1+proj3!$F$33)</f>
-        <v>0.11803393431999383</v>
+        <v>0.16169358531935926</v>
       </c>
       <c r="Y6" s="7">
         <f>M6 + U6 * proj3!$B$25/proj3!$B$17</f>
@@ -4151,11 +4147,11 @@
       </c>
       <c r="Z6" s="7">
         <f t="shared" si="5"/>
-        <v>-8.6749870015545092</v>
+        <v>-6.332612663303288</v>
       </c>
       <c r="AA6" s="7">
         <f t="shared" si="6"/>
-        <v>-77.057227915102601</v>
+        <v>-41.062138748855048</v>
       </c>
       <c r="AB6" s="11"/>
       <c r="AC6" s="11"/>
@@ -4177,7 +4173,7 @@
         <v>32</v>
       </c>
       <c r="H7" s="5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -4201,19 +4197,19 @@
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="1"/>
-        <v>1.9869776164033289E-2</v>
+        <v>1.9927378985098672E-2</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="2"/>
-        <v>7.7633253187835621E-2</v>
+        <v>0.12526492028142416</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="3"/>
-        <v>-3.0398309161293984</v>
+        <v>-5.5517137602901316</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="4"/>
-        <v>-18.1255452018436</v>
+        <v>-20.637428046004331</v>
       </c>
       <c r="U7" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M7*(proj3!$B$31-proj3!$B$32))</f>
@@ -4229,7 +4225,7 @@
       </c>
       <c r="X7" s="7">
         <f>(R7+ W7+proj3!$B$25/proj3!$B$17 * V7)*(1+proj3!$F$33)</f>
-        <v>0.13132469904616462</v>
+        <v>0.18229058283630437</v>
       </c>
       <c r="Y7" s="7">
         <f>M7 + U7 * proj3!$B$25/proj3!$B$17</f>
@@ -4237,11 +4233,11 @@
       </c>
       <c r="Z7" s="7">
         <f t="shared" si="5"/>
-        <v>-8.415753119099783</v>
+        <v>-6.0628268801195198</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="6"/>
-        <v>-78.275414196607727</v>
+        <v>-40.624659675693785</v>
       </c>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
@@ -4262,7 +4258,7 @@
       </c>
       <c r="H8" s="5">
         <f>H3/ H2</f>
-        <v>0.70000000000000018</v>
+        <v>0.76190476190476186</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -4286,19 +4282,19 @@
       </c>
       <c r="Q8" s="7">
         <f t="shared" si="1"/>
-        <v>1.9329924817641241E-2</v>
+        <v>1.9388254895535473E-2</v>
       </c>
       <c r="R8" s="7">
         <f t="shared" si="2"/>
-        <v>7.6391447030614512E-2</v>
+        <v>0.12343605112295625</v>
       </c>
       <c r="S8" s="7">
         <f t="shared" si="3"/>
-        <v>-3.0209935892003328</v>
+        <v>-5.5173107128823711</v>
       </c>
       <c r="T8" s="7">
         <f t="shared" si="4"/>
-        <v>-16.506707874914532</v>
+        <v>-19.003024998596572</v>
       </c>
       <c r="U8" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M8*(proj3!$B$31-proj3!$B$32))</f>
@@ -4314,7 +4310,7 @@
       </c>
       <c r="X8" s="7">
         <f>(R8+ W8+proj3!$B$25/proj3!$B$17 * V8)*(1+proj3!$F$33)</f>
-        <v>0.12993737542269024</v>
+        <v>0.18027510180149592</v>
       </c>
       <c r="Y8" s="7">
         <f>M8 + U8 * proj3!$B$25/proj3!$B$17</f>
@@ -4322,11 +4318,11 @@
       </c>
       <c r="Z8" s="7">
         <f t="shared" si="5"/>
-        <v>-8.4536920143603904</v>
+        <v>-6.093190584838875</v>
       </c>
       <c r="AA8" s="7">
         <f t="shared" si="6"/>
-        <v>-78.500668451086568</v>
+        <v>-40.78214237804508</v>
       </c>
       <c r="AB8" s="11"/>
       <c r="AC8" s="11"/>
@@ -4351,7 +4347,7 @@
       </c>
       <c r="H9" s="5">
         <f>((C4)^2)/H6</f>
-        <v>6.5967841001666665</v>
+        <v>3.5594158813848917</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -4375,19 +4371,19 @@
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="1"/>
-        <v>1.5656033476382718E-2</v>
+        <v>1.5724197970343599E-2</v>
       </c>
       <c r="R9" s="7">
         <f t="shared" si="2"/>
-        <v>6.3653741358226268E-2</v>
+        <v>0.10311848650937638</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="3"/>
-        <v>-2.7662636186372573</v>
+        <v>-5.0520914550514107</v>
       </c>
       <c r="T9" s="7">
         <f t="shared" si="4"/>
-        <v>-14.766263618637257</v>
+        <v>-17.052091455051411</v>
       </c>
       <c r="U9" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M9*(proj3!$B$31-proj3!$B$32))</f>
@@ -4403,7 +4399,7 @@
       </c>
       <c r="X9" s="7">
         <f>(R9+ W9+proj3!$B$25/proj3!$B$17 * V9)*(1+proj3!$F$33)</f>
-        <v>0.11551695044447152</v>
+        <v>0.15774422775620214</v>
       </c>
       <c r="Y9" s="7">
         <f>M9 + U9 * proj3!$B$25/proj3!$B$17</f>
@@ -4411,11 +4407,11 @@
       </c>
       <c r="Z9" s="7">
         <f t="shared" si="5"/>
-        <v>-8.719336222738777</v>
+        <v>-6.3852170356908591</v>
       </c>
       <c r="AA9" s="7">
         <f t="shared" si="6"/>
-        <v>-76.57658404086024</v>
+        <v>-41.065816983771917</v>
       </c>
       <c r="AB9" s="11"/>
       <c r="AC9" s="11"/>
@@ -4459,19 +4455,19 @@
       </c>
       <c r="Q10" s="7">
         <f t="shared" si="1"/>
-        <v>1.230943555139536E-2</v>
+        <v>1.2389612638702818E-2</v>
       </c>
       <c r="R10" s="7">
         <f t="shared" si="2"/>
-        <v>5.0318383442274302E-2</v>
+        <v>8.1430933516464271E-2</v>
       </c>
       <c r="S10" s="7">
         <f t="shared" si="3"/>
-        <v>-2.4551147381321372</v>
+        <v>-4.4838330324419555</v>
       </c>
       <c r="T10" s="7">
         <f t="shared" si="4"/>
-        <v>-13.197971880989236</v>
+        <v>-15.226690175299055</v>
       </c>
       <c r="U10" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M10*(proj3!$B$31-proj3!$B$32))</f>
@@ -4487,7 +4483,7 @@
       </c>
       <c r="X10" s="7">
         <f>(R10+ W10+proj3!$B$25/proj3!$B$17 * V10)*(1+proj3!$F$33)</f>
-        <v>0.10028491839789452</v>
+        <v>0.1335753469772778</v>
       </c>
       <c r="Y10" s="7">
         <f>M10 + U10 * proj3!$B$25/proj3!$B$17</f>
@@ -4495,11 +4491,11 @@
       </c>
       <c r="Z10" s="7">
         <f t="shared" si="5"/>
-        <v>-8.9326288840490093</v>
+        <v>-6.7063869118596742</v>
       </c>
       <c r="AA10" s="7">
         <f t="shared" si="6"/>
-        <v>-71.478182135961049</v>
+        <v>-40.28952319188636</v>
       </c>
       <c r="AB10" s="11"/>
       <c r="AC10" s="11"/>
@@ -4517,7 +4513,7 @@
       </c>
       <c r="H11" s="5">
         <f>2*H4 /(3*PI())</f>
-        <v>2.1109144515459657</v>
+        <v>3.7772773160476496</v>
       </c>
       <c r="I11" s="5">
         <v>2.37</v>
@@ -4543,19 +4539,19 @@
       </c>
       <c r="Q11" s="7">
         <f t="shared" si="1"/>
-        <v>1.005396400761558E-2</v>
+        <v>1.0149091238761409E-2</v>
       </c>
       <c r="R11" s="7">
         <f t="shared" si="2"/>
-        <v>3.7294271487866057E-2</v>
+        <v>5.9404521836758706E-2</v>
       </c>
       <c r="S11" s="7">
         <f t="shared" si="3"/>
-        <v>-2.0678777457115487</v>
+        <v>-3.7766131249439048</v>
       </c>
       <c r="T11" s="7">
         <f t="shared" si="4"/>
-        <v>-11.439306317140108</v>
+        <v>-13.148041696372465</v>
       </c>
       <c r="U11" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M11*(proj3!$B$31-proj3!$B$32))</f>
@@ -4571,7 +4567,7 @@
       </c>
       <c r="X11" s="7">
         <f>(R11+ W11+proj3!$B$25/proj3!$B$17 * V11)*(1+proj3!$F$33)</f>
-        <v>8.515513074514991E-2</v>
+        <v>0.10881309861846504</v>
       </c>
       <c r="Y11" s="7">
         <f>M11 + U11 * proj3!$B$25/proj3!$B$17</f>
@@ -4579,11 +4575,11 @@
       </c>
       <c r="Z11" s="7">
         <f t="shared" si="5"/>
-        <v>-8.8912722267357278</v>
+        <v>-6.9581462027212098</v>
       </c>
       <c r="AA11" s="7">
         <f t="shared" si="6"/>
-        <v>-59.855290399280491</v>
+        <v>-36.657414224966566</v>
       </c>
       <c r="AB11" s="11"/>
       <c r="AC11" s="11"/>
@@ -4620,19 +4616,19 @@
       </c>
       <c r="Q12" s="7">
         <f t="shared" si="1"/>
-        <v>9.4521140298390195E-3</v>
+        <v>9.5549628105605876E-3</v>
       </c>
       <c r="R12" s="7">
         <f t="shared" si="2"/>
-        <v>3.1852682854006623E-2</v>
+        <v>4.9918041692785381E-2</v>
       </c>
       <c r="S12" s="7">
         <f t="shared" si="3"/>
-        <v>-1.8678750121685168</v>
+        <v>-3.4113434903682087</v>
       </c>
       <c r="T12" s="7">
         <f t="shared" si="4"/>
-        <v>-10.553589297882796</v>
+        <v>-12.097057776082488</v>
       </c>
       <c r="U12" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M12*(proj3!$B$31-proj3!$B$32))</f>
@@ -4648,7 +4644,7 @@
       </c>
       <c r="X12" s="7">
         <f>(R12+ W12+proj3!$B$25/proj3!$B$17 * V12)*(1+proj3!$F$33)</f>
-        <v>7.8718015516894849E-2</v>
+        <v>9.8047949474388121E-2</v>
       </c>
       <c r="Y12" s="7">
         <f>M12 + U12 * proj3!$B$25/proj3!$B$17</f>
@@ -4656,11 +4652,11 @@
       </c>
       <c r="Z12" s="7">
         <f t="shared" si="5"/>
-        <v>-8.7085018422589915</v>
+        <v>-6.9916401803682771</v>
       </c>
       <c r="AA12" s="7">
         <f t="shared" si="6"/>
-        <v>-51.988164102794677</v>
+        <v>-33.5101000229823</v>
       </c>
       <c r="AB12" s="11"/>
       <c r="AC12" s="11"/>
@@ -4680,7 +4676,7 @@
       </c>
       <c r="H13" s="5">
         <f>0.239*H7</f>
-        <v>0.35849999999999999</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -4704,19 +4700,19 @@
       </c>
       <c r="Q13" s="7">
         <f t="shared" si="1"/>
-        <v>8.9865251771255282E-3</v>
+        <v>9.097144955396758E-3</v>
       </c>
       <c r="R13" s="7">
         <f t="shared" si="2"/>
-        <v>2.7012978173735405E-2</v>
+        <v>4.1423389795914867E-2</v>
       </c>
       <c r="S13" s="7">
         <f t="shared" si="3"/>
-        <v>-1.6665914826070818</v>
+        <v>-3.0437347082952737</v>
       </c>
       <c r="T13" s="7">
         <f t="shared" si="4"/>
-        <v>-9.6665914826070818</v>
+        <v>-11.043734708295274</v>
       </c>
       <c r="U13" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M13*(proj3!$B$31-proj3!$B$32))</f>
@@ -4732,7 +4728,7 @@
       </c>
       <c r="X13" s="7">
         <f>(R13+ W13+proj3!$B$25/proj3!$B$17 * V13)*(1+proj3!$F$33)</f>
-        <v>7.2922399221151818E-2</v>
+        <v>8.8341539656883836E-2</v>
       </c>
       <c r="Y13" s="7">
         <f>M13 + U13 * proj3!$B$25/proj3!$B$17</f>
@@ -4740,11 +4736,11 @@
       </c>
       <c r="Z13" s="7">
         <f t="shared" si="5"/>
-        <v>-8.4121733200865094</v>
+        <v>-6.943911817107093</v>
       </c>
       <c r="AA13" s="7">
         <f t="shared" si="6"/>
-        <v>-43.409580127003416</v>
+        <v>-29.578595956461797</v>
       </c>
       <c r="AB13" s="11"/>
       <c r="AC13" s="11"/>
@@ -4768,7 +4764,7 @@
       </c>
       <c r="H14" s="5">
         <f>0.006*H7</f>
-        <v>9.0000000000000011E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -4792,19 +4788,19 @@
       </c>
       <c r="Q14" s="7">
         <f t="shared" si="1"/>
-        <v>8.5110655019087177E-3</v>
+        <v>8.6294874796283959E-3</v>
       </c>
       <c r="R14" s="7">
         <f t="shared" si="2"/>
-        <v>2.2647045457975752E-2</v>
+        <v>3.3807525138802919E-2</v>
       </c>
       <c r="S14" s="7">
         <f t="shared" si="3"/>
-        <v>-1.4644997648720184</v>
+        <v>-2.674649913401812</v>
       </c>
       <c r="T14" s="7">
         <f t="shared" si="4"/>
-        <v>-8.7787854791577278</v>
+        <v>-9.9889356276875212</v>
       </c>
       <c r="U14" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M14*(proj3!$B$31-proj3!$B$32))</f>
@@ -4820,7 +4816,7 @@
       </c>
       <c r="X14" s="7">
         <f>(R14+ W14+proj3!$B$25/proj3!$B$17 * V14)*(1+proj3!$F$33)</f>
-        <v>6.7632673182109679E-2</v>
+        <v>7.9574386440594738E-2</v>
       </c>
       <c r="Y14" s="7">
         <f>M14 + U14 * proj3!$B$25/proj3!$B$17</f>
@@ -4828,11 +4824,11 @@
       </c>
       <c r="Z14" s="7">
         <f t="shared" si="5"/>
-        <v>-8.0000730352975946</v>
+        <v>-6.7995035743469625</v>
       </c>
       <c r="AA14" s="7">
         <f t="shared" si="6"/>
-        <v>-34.628877075801789</v>
+        <v>-25.015254053523069</v>
       </c>
       <c r="AB14" s="11"/>
       <c r="AC14" s="11"/>
@@ -4878,19 +4874,19 @@
       </c>
       <c r="Q15" s="7">
         <f t="shared" si="1"/>
-        <v>7.9681452410872641E-3</v>
+        <v>8.0943875391511193E-3</v>
       </c>
       <c r="R15" s="7">
         <f t="shared" si="2"/>
-        <v>1.8708577161275275E-2</v>
+        <v>2.7033574394907445E-2</v>
       </c>
       <c r="S15" s="7">
         <f t="shared" si="3"/>
-        <v>-1.2619386816754596</v>
+        <v>-2.3047079054714805</v>
       </c>
       <c r="T15" s="7">
         <f t="shared" si="4"/>
-        <v>-7.89051011024688</v>
+        <v>-8.9332793340429006</v>
       </c>
       <c r="U15" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M15*(proj3!$B$31-proj3!$B$32))</f>
@@ -4906,7 +4902,7 @@
       </c>
       <c r="X15" s="7">
         <f>(R15+ W15+proj3!$B$25/proj3!$B$17 * V15)*(1+proj3!$F$33)</f>
-        <v>6.2800338350301257E-2</v>
+        <v>7.1708085390287696E-2</v>
       </c>
       <c r="Y15" s="7">
         <f>M15 + U15 * proj3!$B$25/proj3!$B$17</f>
@@ -4914,11 +4910,11 @@
       </c>
       <c r="Z15" s="7">
         <f t="shared" si="5"/>
-        <v>-7.4606080203862311</v>
+        <v>-6.533833743142794</v>
       </c>
       <c r="AA15" s="7">
         <f t="shared" si="6"/>
-        <v>-26.078622753275848</v>
+        <v>-20.001951286814325</v>
       </c>
       <c r="AB15" s="11"/>
       <c r="AC15" s="11"/>
@@ -4959,19 +4955,19 @@
       </c>
       <c r="Q16" s="7">
         <f t="shared" si="1"/>
-        <v>6.8640609922672345E-3</v>
+        <v>7.0058234799979004E-3</v>
       </c>
       <c r="R16" s="7">
         <f t="shared" si="2"/>
-        <v>1.2359964048372397E-2</v>
+        <v>1.6308912488956176E-2</v>
       </c>
       <c r="S16" s="7">
         <f t="shared" si="3"/>
-        <v>-0.85993642448330532</v>
+        <v>-1.5705218522014133</v>
       </c>
       <c r="T16" s="7">
         <f t="shared" si="4"/>
-        <v>-6.1170792816261557</v>
+        <v>-6.8276647093442637</v>
       </c>
       <c r="U16" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M16*(proj3!$B$31-proj3!$B$32))</f>
@@ -4987,7 +4983,7 @@
       </c>
       <c r="X16" s="7">
         <f>(R16+ W16+proj3!$B$25/proj3!$B$17 * V16)*(1+proj3!$F$33)</f>
-        <v>5.4784765845284703E-2</v>
+        <v>5.9010140676709344E-2</v>
       </c>
       <c r="Y16" s="7">
         <f>M16 + U16 * proj3!$B$25/proj3!$B$17</f>
@@ -4995,11 +4991,11 @@
       </c>
       <c r="Z16" s="7">
         <f t="shared" si="5"/>
-        <v>-5.9244703514173009</v>
+        <v>-5.5002532994779472</v>
       </c>
       <c r="AA16" s="7">
         <f t="shared" si="6"/>
-        <v>-11.392220992238164</v>
+        <v>-9.81916867939238</v>
       </c>
       <c r="AB16" s="11"/>
       <c r="AC16" s="11"/>
@@ -5011,7 +5007,7 @@
       </c>
       <c r="B17" s="5">
         <f>B14 *H7/B15</f>
-        <v>2535934.2915811082</v>
+        <v>3381245.7221081443</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -5041,19 +5037,19 @@
       </c>
       <c r="Q17" s="7">
         <f t="shared" si="1"/>
-        <v>6.3627583772379089E-3</v>
+        <v>6.5145711117251259E-3</v>
       </c>
       <c r="R17" s="7">
         <f t="shared" si="2"/>
-        <v>9.5225902582855293E-3</v>
+        <v>1.1525451801628683E-2</v>
       </c>
       <c r="S17" s="7">
         <f t="shared" si="3"/>
-        <v>-0.59961603096958072</v>
+        <v>-1.0950926751751844</v>
       </c>
       <c r="T17" s="7">
         <f t="shared" si="4"/>
-        <v>-4.9424731738267207</v>
+        <v>-5.4379498180323242</v>
       </c>
       <c r="U17" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M17*(proj3!$B$31-proj3!$B$32))</f>
@@ -5069,7 +5065,7 @@
       </c>
       <c r="X17" s="7">
         <f>(R17+ W17+proj3!$B$25/proj3!$B$17 * V17)*(1+proj3!$F$33)</f>
-        <v>5.0960126851079882E-2</v>
+        <v>5.3103188702457053E-2</v>
       </c>
       <c r="Y17" s="7">
         <f>M17 + U17 * proj3!$B$25/proj3!$B$17</f>
@@ -5077,11 +5073,11 @@
       </c>
       <c r="Z17" s="7">
         <f t="shared" si="5"/>
-        <v>-4.5398111927727944</v>
+        <v>-4.3566000444894089</v>
       </c>
       <c r="AA17" s="7">
         <f t="shared" si="6"/>
-        <v>-4.7680837402826519</v>
+        <v>-4.3910024032351282</v>
       </c>
       <c r="AB17" s="11"/>
       <c r="AC17" s="11"/>
@@ -5124,19 +5120,19 @@
       </c>
       <c r="Q18" s="7">
         <f t="shared" si="1"/>
-        <v>6.1169209258261515E-3</v>
+        <v>6.2784672483895592E-3</v>
       </c>
       <c r="R18" s="7">
         <f t="shared" si="2"/>
-        <v>7.8086220669495035E-3</v>
+        <v>8.5918603605836374E-3</v>
       </c>
       <c r="S18" s="7">
         <f t="shared" si="3"/>
-        <v>-0.34749769600005148</v>
+        <v>-0.6346431080479481</v>
       </c>
       <c r="T18" s="7">
         <f t="shared" si="4"/>
-        <v>-3.7760691245714817</v>
+        <v>-4.0632145366193786</v>
       </c>
       <c r="U18" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M18*(proj3!$B$31-proj3!$B$32))</f>
@@ -5152,7 +5148,7 @@
       </c>
       <c r="X18" s="7">
         <f>(R18+ W18+proj3!$B$25/proj3!$B$17 * V18)*(1+proj3!$F$33)</f>
-        <v>4.8364649990114743E-2</v>
+        <v>4.9202714964303264E-2</v>
       </c>
       <c r="Y18" s="7">
         <f>M18 + U18 * proj3!$B$25/proj3!$B$17</f>
@@ -5160,11 +5156,11 @@
       </c>
       <c r="Z18" s="7">
         <f t="shared" si="5"/>
-        <v>-2.9166997947862212</v>
+        <v>-2.8670199358596031</v>
       </c>
       <c r="AA18" s="7">
         <f t="shared" si="6"/>
-        <v>-1.2000607797845066</v>
+        <v>-1.1595279081046754</v>
       </c>
       <c r="AB18" s="11"/>
       <c r="AC18" s="11"/>
@@ -5182,7 +5178,7 @@
       </c>
       <c r="H19" s="11">
         <f>H18*(B17/10000000)^(0.11)</f>
-        <v>5.4418817621892396E-3</v>
+        <v>5.6168440048232722E-3</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -5206,19 +5202,19 @@
       </c>
       <c r="Q19" s="7">
         <f t="shared" si="1"/>
-        <v>5.9444340120149665E-3</v>
+        <v>6.1184734775255158E-3</v>
       </c>
       <c r="R19" s="7">
         <f t="shared" si="2"/>
-        <v>6.8972064991646683E-3</v>
+        <v>7.0741871878086159E-3</v>
       </c>
       <c r="S19" s="7">
         <f t="shared" si="3"/>
-        <v>2.3901672240455016E-2</v>
+        <v>4.3652178799549468E-2</v>
       </c>
       <c r="T19" s="7">
         <f t="shared" si="4"/>
-        <v>-2.033241184902395</v>
+        <v>-2.0134906783433002</v>
       </c>
       <c r="U19" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M19*(proj3!$B$31-proj3!$B$32))</f>
@@ -5234,7 +5230,7 @@
       </c>
       <c r="X19" s="7">
         <f>(R19+ W19+proj3!$B$25/proj3!$B$17 * V19)*(1+proj3!$F$33)</f>
-        <v>4.6410003404017047E-2</v>
+        <v>4.6599372740866077E-2</v>
       </c>
       <c r="Y19" s="7">
         <f>M19 + U19 * proj3!$B$25/proj3!$B$17</f>
@@ -5242,11 +5238,11 @@
       </c>
       <c r="Z19" s="7">
         <f t="shared" si="5"/>
-        <v>-0.17380189893681125</v>
+        <v>-0.17309560723353468</v>
       </c>
       <c r="AA19" s="7">
         <f t="shared" si="6"/>
-        <v>-2.4365490122166866E-4</v>
+        <v>-2.4167860791458922E-4</v>
       </c>
       <c r="AB19" s="11"/>
       <c r="AC19" s="11"/>
@@ -5287,19 +5283,19 @@
       </c>
       <c r="Q20" s="7">
         <f t="shared" si="1"/>
-        <v>5.8693090665680198E-3</v>
+        <v>6.0360354431953254E-3</v>
       </c>
       <c r="R20" s="7">
         <f t="shared" si="2"/>
-        <v>7.0983638735966758E-3</v>
+        <v>7.4993797789720904E-3</v>
       </c>
       <c r="S20" s="7">
         <f t="shared" si="3"/>
-        <v>0.2133245015501625</v>
+        <v>0.38959948870151462</v>
       </c>
       <c r="T20" s="7">
         <f t="shared" si="4"/>
-        <v>-1.1581040698783973</v>
+        <v>-0.98182908272704528</v>
       </c>
       <c r="U20" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M20*(proj3!$B$31-proj3!$B$32))</f>
@@ -5315,7 +5311,7 @@
       </c>
       <c r="X20" s="7">
         <f>(R20+ W20+proj3!$B$25/proj3!$B$17 * V20)*(1+proj3!$F$33)</f>
-        <v>4.7153243616925355E-2</v>
+        <v>4.7582330635677045E-2</v>
       </c>
       <c r="Y20" s="7">
         <f>M20 + U20 * proj3!$B$25/proj3!$B$17</f>
@@ -5323,11 +5319,11 @@
       </c>
       <c r="Z20" s="7">
         <f t="shared" si="5"/>
-        <v>1.2674977380328978</v>
+        <v>1.2560677215032061</v>
       </c>
       <c r="AA20" s="7">
         <f t="shared" si="6"/>
-        <v>9.6018109659344097E-2</v>
+        <v>9.4294177391616371E-2</v>
       </c>
       <c r="AB20" s="11"/>
       <c r="AC20" s="11"/>
@@ -5369,19 +5365,19 @@
       </c>
       <c r="Q21" s="7">
         <f t="shared" si="1"/>
-        <v>5.6786491397739667E-3</v>
+        <v>5.8352539540807999E-3</v>
       </c>
       <c r="R21" s="7">
         <f t="shared" si="2"/>
-        <v>8.018005120966256E-3</v>
+        <v>9.3386234343328725E-3</v>
       </c>
       <c r="S21" s="7">
         <f t="shared" si="3"/>
-        <v>0.47549210300945621</v>
+        <v>0.8684022644746735</v>
       </c>
       <c r="T21" s="7">
         <f t="shared" si="4"/>
-        <v>1.8349245866601194E-2</v>
+        <v>0.41125940733181848</v>
       </c>
       <c r="U21" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M21*(proj3!$B$31-proj3!$B$32))</f>
@@ -5397,7 +5393,7 @@
       </c>
       <c r="X21" s="7">
         <f>(R21+ W21+proj3!$B$25/proj3!$B$17 * V21)*(1+proj3!$F$33)</f>
-        <v>4.8870112083085337E-2</v>
+        <v>5.0283173678387624E-2</v>
       </c>
       <c r="Y21" s="7">
         <f>M21 + U21 * proj3!$B$25/proj3!$B$17</f>
@@ -5405,11 +5401,11 @@
       </c>
       <c r="Z21" s="7">
         <f t="shared" si="5"/>
-        <v>3.1440379290057403</v>
+        <v>3.0556839344852773</v>
       </c>
       <c r="AA21" s="7">
         <f t="shared" si="6"/>
-        <v>1.5188212507402237</v>
+        <v>1.4346566423704075</v>
       </c>
       <c r="AB21" s="11"/>
       <c r="AC21" s="11"/>
@@ -5446,19 +5442,19 @@
       </c>
       <c r="Q22" s="7">
         <f t="shared" si="1"/>
-        <v>5.5025677574034194E-3</v>
+        <v>5.6499680941891998E-3</v>
       </c>
       <c r="R22" s="7">
         <f t="shared" si="2"/>
-        <v>9.5853991583885363E-3</v>
+        <v>1.2356732993554675E-2</v>
       </c>
       <c r="S22" s="7">
         <f t="shared" si="3"/>
-        <v>0.71390547418430295</v>
+        <v>1.3038221381148472</v>
       </c>
       <c r="T22" s="7">
         <f t="shared" si="4"/>
-        <v>1.0567626170414439</v>
+        <v>1.6466792809719881</v>
       </c>
       <c r="U22" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M22*(proj3!$B$31-proj3!$B$32))</f>
@@ -5474,7 +5470,7 @@
       </c>
       <c r="X22" s="7">
         <f>(R22+ W22+proj3!$B$25/proj3!$B$17 * V22)*(1+proj3!$F$33)</f>
-        <v>5.1215771147734873E-2</v>
+        <v>5.418109835136263E-2</v>
       </c>
       <c r="Y22" s="7">
         <f>M22 + U22 * proj3!$B$25/proj3!$B$17</f>
@@ -5482,11 +5478,11 @@
       </c>
       <c r="Z22" s="7">
         <f t="shared" si="5"/>
-        <v>4.66703691634262</v>
+        <v>4.4116103570909333</v>
       </c>
       <c r="AA22" s="7">
         <f t="shared" si="6"/>
-        <v>5.2062788425832824</v>
+        <v>4.6519950898390015</v>
       </c>
       <c r="AB22" s="11"/>
       <c r="AC22" s="11"/>
@@ -5527,19 +5523,19 @@
       </c>
       <c r="Q23" s="7">
         <f t="shared" si="1"/>
-        <v>5.4233171160383556E-3</v>
+        <v>5.5626936310165052E-3</v>
       </c>
       <c r="R23" s="7">
         <f t="shared" si="2"/>
-        <v>1.1596211917647717E-2</v>
+        <v>1.6109661522180893E-2</v>
       </c>
       <c r="S23" s="7">
         <f t="shared" si="3"/>
-        <v>0.92173763005502651</v>
+        <v>1.6833908284179964</v>
       </c>
       <c r="T23" s="7">
         <f t="shared" si="4"/>
-        <v>1.9503090586264564</v>
+        <v>2.7119622569894264</v>
       </c>
       <c r="U23" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M23*(proj3!$B$31-proj3!$B$32))</f>
@@ -5555,7 +5551,7 @@
       </c>
       <c r="X23" s="7">
         <f>(R23+ W23+proj3!$B$25/proj3!$B$17 * V23)*(1+proj3!$F$33)</f>
-        <v>5.3951763212552267E-2</v>
+        <v>5.8781154289402768E-2</v>
       </c>
       <c r="Y23" s="7">
         <f>M23 + U23 * proj3!$B$25/proj3!$B$17</f>
@@ -5563,11 +5559,11 @@
       </c>
       <c r="Z23" s="7">
         <f t="shared" si="5"/>
-        <v>5.8098396973279849</v>
+        <v>5.3325100441186066</v>
       </c>
       <c r="AA23" s="7">
         <f t="shared" si="6"/>
-        <v>10.580302667331374</v>
+        <v>8.9131898391461224</v>
       </c>
       <c r="AB23" s="11"/>
       <c r="AC23" s="11"/>
@@ -5604,19 +5600,19 @@
       </c>
       <c r="Q24" s="7">
         <f t="shared" si="1"/>
-        <v>5.5220685923252667E-3</v>
+        <v>5.6495567556489636E-3</v>
       </c>
       <c r="R24" s="7">
         <f t="shared" si="2"/>
-        <v>1.5768143984692975E-2</v>
+        <v>2.3680431731208811E-2</v>
       </c>
       <c r="S24" s="7">
         <f t="shared" si="3"/>
-        <v>1.2296684158239504</v>
+        <v>2.2457719699148533</v>
       </c>
       <c r="T24" s="7">
         <f t="shared" si="4"/>
-        <v>3.2868112729668102</v>
+        <v>4.3029148270577133</v>
       </c>
       <c r="U24" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M24*(proj3!$B$31-proj3!$B$32))</f>
@@ -5632,7 +5628,7 @@
       </c>
       <c r="X24" s="7">
         <f>(R24+ W24+proj3!$B$25/proj3!$B$17 * V24)*(1+proj3!$F$33)</f>
-        <v>5.9284419695124664E-2</v>
+        <v>6.7750567583896595E-2</v>
       </c>
       <c r="Y24" s="7">
         <f>M24 + U24 * proj3!$B$25/proj3!$B$17</f>
@@ -5640,11 +5636,11 @@
       </c>
       <c r="Z24" s="7">
         <f t="shared" si="5"/>
-        <v>7.1472717774346686</v>
+        <v>6.2541447967038071</v>
       </c>
       <c r="AA24" s="7">
         <f t="shared" si="6"/>
-        <v>21.645193020009344</v>
+        <v>16.573595437002687</v>
       </c>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
@@ -5664,7 +5660,7 @@
       </c>
       <c r="H25" s="5">
         <f>0.23*(H9/H16)^3-0.103*(H9/H16)^2+0.25*(H9/H16)</f>
-        <v>0.50601244047748251</v>
+        <v>0.17153003605481118</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -5688,19 +5684,19 @@
       </c>
       <c r="Q25" s="7">
         <f t="shared" si="1"/>
-        <v>5.7821136565607747E-3</v>
+        <v>5.9007573629641869E-3</v>
       </c>
       <c r="R25" s="7">
         <f t="shared" si="2"/>
-        <v>1.9814870151578776E-2</v>
+        <v>3.0889136161155861E-2</v>
       </c>
       <c r="S25" s="7">
         <f t="shared" si="3"/>
-        <v>1.4587565727294323</v>
+        <v>2.6641609882853503</v>
       </c>
       <c r="T25" s="7">
         <f t="shared" si="4"/>
-        <v>4.3158994298722924</v>
+        <v>5.5213038454282106</v>
       </c>
       <c r="U25" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M25*(proj3!$B$31-proj3!$B$32))</f>
@@ -5716,7 +5712,7 @@
       </c>
       <c r="X25" s="7">
         <f>(R25+ W25+proj3!$B$25/proj3!$B$17 * V25)*(1+proj3!$F$33)</f>
-        <v>6.4262847939001444E-2</v>
+        <v>7.6112312569248927E-2</v>
       </c>
       <c r="Y25" s="7">
         <f>M25 + U25 * proj3!$B$25/proj3!$B$17</f>
@@ -5724,11 +5720,11 @@
       </c>
       <c r="Z25" s="7">
         <f t="shared" si="5"/>
-        <v>7.8701598618372914</v>
+        <v>6.6449023736695709</v>
       </c>
       <c r="AA25" s="7">
         <f t="shared" si="6"/>
-        <v>31.326410190831758</v>
+        <v>22.33164584032702</v>
       </c>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
@@ -5746,7 +5742,7 @@
       </c>
       <c r="H26" s="5">
         <f>-0.18*H8^5+1.52*H8^4-3.51*H8^3+3.5*H8^2-1.33*H8+0.17</f>
-        <v>8.4769400000000189E-2</v>
+        <v>0.10198659876433055</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -5770,19 +5766,19 @@
       </c>
       <c r="Q26" s="7">
         <f t="shared" si="1"/>
-        <v>6.0431935212442852E-3</v>
+        <v>6.1557898031861461E-3</v>
       </c>
       <c r="R26" s="7">
         <f t="shared" si="2"/>
-        <v>2.3036589664283388E-2</v>
+        <v>3.6583935275715726E-2</v>
       </c>
       <c r="S26" s="7">
         <f t="shared" si="3"/>
-        <v>1.6153963004604455</v>
+        <v>2.9502357588385912</v>
       </c>
       <c r="T26" s="7">
         <f t="shared" si="4"/>
-        <v>5.0439677290318752</v>
+        <v>6.3788071874100218</v>
       </c>
       <c r="U26" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M26*(proj3!$B$31-proj3!$B$32))</f>
@@ -5798,7 +5794,7 @@
       </c>
       <c r="X26" s="7">
         <f>(R26+ W26+proj3!$B$25/proj3!$B$17 * V26)*(1+proj3!$F$33)</f>
-        <v>6.8154516146949923E-2</v>
+        <v>8.2650175951182528E-2</v>
       </c>
       <c r="Y26" s="7">
         <f>M26 + U26 * proj3!$B$25/proj3!$B$17</f>
@@ -5806,11 +5802,11 @@
       </c>
       <c r="Z26" s="7">
         <f t="shared" si="5"/>
-        <v>8.2437963920496014</v>
+        <v>6.7979523073970336</v>
       </c>
       <c r="AA26" s="7">
         <f t="shared" si="6"/>
-        <v>38.1835593606001</v>
+        <v>25.964389922120031</v>
       </c>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
@@ -5847,19 +5843,19 @@
       </c>
       <c r="Q27" s="7">
         <f t="shared" si="1"/>
-        <v>6.8771821183495428E-3</v>
+        <v>6.9757958799166976E-3</v>
       </c>
       <c r="R27" s="7">
         <f t="shared" si="2"/>
-        <v>3.187128302222382E-2</v>
+        <v>5.2104131954263666E-2</v>
       </c>
       <c r="S27" s="7">
         <f t="shared" si="3"/>
-        <v>1.9775700156366063</v>
+        <v>3.6116820213560747</v>
       </c>
       <c r="T27" s="7">
         <f t="shared" si="4"/>
-        <v>6.7775700156366057</v>
+        <v>8.411682021356075</v>
       </c>
       <c r="U27" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M27*(proj3!$B$31-proj3!$B$32))</f>
@@ -5875,7 +5871,7 @@
       </c>
       <c r="X27" s="7">
         <f>(R27+ W27+proj3!$B$25/proj3!$B$17 * V27)*(1+proj3!$F$33)</f>
-        <v>7.86385217389583E-2</v>
+        <v>0.10028767009624094</v>
       </c>
       <c r="Y27" s="7">
         <f>M27 + U27 * proj3!$B$25/proj3!$B$17</f>
@@ -5883,11 +5879,11 @@
       </c>
       <c r="Z27" s="7">
         <f t="shared" si="5"/>
-        <v>8.7940010592555424</v>
+        <v>6.8956357527006746</v>
       </c>
       <c r="AA27" s="7">
         <f t="shared" si="6"/>
-        <v>53.480428924815321</v>
+        <v>32.882927885283436</v>
       </c>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
@@ -5905,7 +5901,7 @@
       </c>
       <c r="H28" s="5">
         <f>H25*H26/1.7</f>
-        <v>2.5231982924595296E-2</v>
+        <v>1.02904499783254E-2</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -5929,19 +5925,19 @@
       </c>
       <c r="Q28" s="7">
         <f t="shared" si="1"/>
-        <v>7.9136948419598879E-3</v>
+        <v>8.0002519962928797E-3</v>
       </c>
       <c r="R28" s="7">
         <f t="shared" si="2"/>
-        <v>4.1101514459634295E-2</v>
+        <v>6.8183415167892544E-2</v>
       </c>
       <c r="S28" s="7">
         <f t="shared" si="3"/>
-        <v>2.289858939049541</v>
+        <v>4.1820225307898502</v>
       </c>
       <c r="T28" s="7">
         <f t="shared" si="4"/>
-        <v>8.2327160819066805</v>
+        <v>10.124879673646991</v>
       </c>
       <c r="U28" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M28*(proj3!$B$31-proj3!$B$32))</f>
@@ -5957,7 +5953,7 @@
       </c>
       <c r="X28" s="7">
         <f>(R28+ W28+proj3!$B$25/proj3!$B$17 * V28)*(1+proj3!$F$33)</f>
-        <v>8.9407462410752675E-2</v>
+        <v>0.118385096168589</v>
       </c>
       <c r="Y28" s="7">
         <f>M28 + U28 * proj3!$B$25/proj3!$B$17</f>
@@ -5965,11 +5961,11 @@
       </c>
       <c r="Z28" s="7">
         <f t="shared" si="5"/>
-        <v>8.9855885133609359</v>
+        <v>6.7861470172118548</v>
       </c>
       <c r="AA28" s="7">
         <f t="shared" si="6"/>
-        <v>64.865437044743373</v>
+        <v>36.997026750425363</v>
       </c>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
@@ -6006,19 +6002,19 @@
       </c>
       <c r="Q29" s="7">
         <f t="shared" si="1"/>
-        <v>8.7686475291452858E-3</v>
+        <v>8.8474161120322813E-3</v>
       </c>
       <c r="R29" s="7">
         <f t="shared" si="2"/>
-        <v>4.7887190478587367E-2</v>
+        <v>7.9927464744323468E-2</v>
       </c>
       <c r="S29" s="7">
         <f t="shared" si="3"/>
-        <v>2.491597665753909</v>
+        <v>4.5504626499706031</v>
       </c>
       <c r="T29" s="7">
         <f t="shared" si="4"/>
-        <v>9.1201690943253393</v>
+        <v>11.179034078542033</v>
       </c>
       <c r="U29" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M29*(proj3!$B$31-proj3!$B$32))</f>
@@ -6034,7 +6030,7 @@
       </c>
       <c r="X29" s="7">
         <f>(R29+ W29+proj3!$B$25/proj3!$B$17 * V29)*(1+proj3!$F$33)</f>
-        <v>9.7246572906923873E-2</v>
+        <v>0.13152966637126151</v>
       </c>
       <c r="Y29" s="7">
         <f>M29 + U29 * proj3!$B$25/proj3!$B$17</f>
@@ -6042,11 +6038,11 @@
       </c>
       <c r="Z29" s="7">
         <f t="shared" si="5"/>
-        <v>9.0041404057803849</v>
+        <v>6.6572190182808804</v>
       </c>
       <c r="AA29" s="7">
         <f t="shared" si="6"/>
-        <v>70.990638253829474</v>
+        <v>38.806301550943175</v>
       </c>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
@@ -6064,7 +6060,7 @@
       </c>
       <c r="H30" s="5">
         <f>0.0537*(H9/H16)-0.005</f>
-        <v>5.7039808437644481E-2</v>
+        <v>2.8474716782901695E-2</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -6088,19 +6084,19 @@
       </c>
       <c r="Q30" s="7">
         <f t="shared" si="1"/>
-        <v>1.0934635921256852E-2</v>
+        <v>1.0996770972873752E-2</v>
       </c>
       <c r="R30" s="7">
         <f t="shared" si="2"/>
-        <v>6.4394698620183335E-2</v>
+        <v>0.1084273824792213</v>
       </c>
       <c r="S30" s="7">
         <f t="shared" si="3"/>
-        <v>2.9224375755234675</v>
+        <v>5.3373155774996803</v>
       </c>
       <c r="T30" s="7">
         <f t="shared" si="4"/>
-        <v>10.922437575523468</v>
+        <v>13.33731557749968</v>
       </c>
       <c r="U30" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M30*(proj3!$B$31-proj3!$B$32))</f>
@@ -6116,7 +6112,7 @@
       </c>
       <c r="X30" s="7">
         <f>(R30+ W30+proj3!$B$25/proj3!$B$17 * V30)*(1+proj3!$F$33)</f>
-        <v>0.11614972424567534</v>
+        <v>0.16326469597484597</v>
       </c>
       <c r="Y30" s="7">
         <f>M30 + U30 * proj3!$B$25/proj3!$B$17</f>
@@ -6124,11 +6120,11 @@
       </c>
       <c r="Z30" s="7">
         <f t="shared" si="5"/>
-        <v>8.8670603717698615</v>
+        <v>6.3082016041575919</v>
       </c>
       <c r="AA30" s="7">
         <f t="shared" si="6"/>
-        <v>80.976160213776765</v>
+        <v>40.983493677309212</v>
       </c>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
@@ -6146,7 +6142,7 @@
       </c>
       <c r="H31" s="5">
         <f>-0.43*H8^5+1.83*H8^4-3.06*H8^3+2.56*H8^2-H8+0.148</f>
-        <v>1.9932900000000003E-2</v>
+        <v>2.5051424536268713E-2</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -6170,19 +6166,19 @@
       </c>
       <c r="Q31" s="7">
         <f t="shared" si="1"/>
-        <v>1.2784826667452657E-2</v>
+        <v>1.2833367210340134E-2</v>
       </c>
       <c r="R31" s="7">
         <f t="shared" si="2"/>
-        <v>7.9661244823534039E-2</v>
+        <v>0.13491467991083125</v>
       </c>
       <c r="S31" s="7">
         <f t="shared" si="3"/>
-        <v>3.2745610554531455</v>
+        <v>5.9804068621083628</v>
       </c>
       <c r="T31" s="7">
         <f t="shared" si="4"/>
-        <v>12.417418198310287</v>
+        <v>15.123264004965502</v>
       </c>
       <c r="U31" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M31*(proj3!$B$31-proj3!$B$32))</f>
@@ -6198,7 +6194,7 @@
       </c>
       <c r="X31" s="7">
         <f>(R31+ W31+proj3!$B$25/proj3!$B$17 * V31)*(1+proj3!$F$33)</f>
-        <v>0.1335033147051678</v>
+        <v>0.19262449024857584</v>
       </c>
       <c r="Y31" s="7">
         <f>M31 + U31 * proj3!$B$25/proj3!$B$17</f>
@@ -6206,11 +6202,11 @@
       </c>
       <c r="Z31" s="7">
         <f t="shared" si="5"/>
-        <v>8.6589827005432305</v>
+        <v>6.0013287563042539</v>
       </c>
       <c r="AA31" s="7">
         <f t="shared" si="6"/>
-        <v>86.674763381606098</v>
+        <v>41.634538724504843</v>
       </c>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
@@ -6228,7 +6224,7 @@
       </c>
       <c r="H32" s="5">
         <f>(-2.2*0.0000001 *(H9^3)+0.0000001 *(H9^2)+1.6*10^(-5))*H35^3+1</f>
-        <v>0.99984669076426813</v>
+        <v>1.0000263097837243</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -6252,19 +6248,19 @@
       </c>
       <c r="Q32" s="7">
         <f t="shared" si="1"/>
-        <v>1.4275272831351295E-2</v>
+        <v>1.4313033697529723E-2</v>
       </c>
       <c r="R32" s="7">
         <f t="shared" si="2"/>
-        <v>9.2873921705020859E-2</v>
+        <v>0.15793232723572856</v>
       </c>
       <c r="S32" s="7">
         <f t="shared" si="3"/>
-        <v>3.5537750639073957</v>
+        <v>6.4903418866441944</v>
       </c>
       <c r="T32" s="7">
         <f t="shared" si="4"/>
-        <v>13.725203635335895</v>
+        <v>16.661770458072695</v>
       </c>
       <c r="U32" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M32*(proj3!$B$31-proj3!$B$32))</f>
@@ -6280,7 +6276,7 @@
       </c>
       <c r="X32" s="7">
         <f>(R32+ W32+proj3!$B$25/proj3!$B$17 * V32)*(1+proj3!$F$33)</f>
-        <v>0.14845149840956146</v>
+        <v>0.21806399232741872</v>
       </c>
       <c r="Y32" s="7">
         <f>M32 + U32 * proj3!$B$25/proj3!$B$17</f>
@@ -6288,11 +6284,11 @@
       </c>
       <c r="Z32" s="7">
         <f t="shared" si="5"/>
-        <v>8.4606091697165677</v>
+        <v>5.759731789264209</v>
       </c>
       <c r="AA32" s="7">
         <f t="shared" si="6"/>
-        <v>89.906167810529709</v>
+        <v>41.666856778067519</v>
       </c>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
@@ -6310,7 +6306,7 @@
       </c>
       <c r="H33" s="5">
         <f>H32*H31*H30/0.048</f>
-        <v>2.3683218537277329E-2</v>
+        <v>1.4861478881143397E-2</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -6334,19 +6330,19 @@
       </c>
       <c r="Q33" s="7">
         <f t="shared" si="1"/>
-        <v>1.519132562638937E-2</v>
+        <v>1.5223765786895263E-2</v>
       </c>
       <c r="R33" s="7">
         <f t="shared" si="2"/>
-        <v>9.9929279790266473E-2</v>
+        <v>0.1701231853423146</v>
       </c>
       <c r="S33" s="7">
         <f t="shared" si="3"/>
-        <v>3.6915914009581772</v>
+        <v>6.7420390618843955</v>
       </c>
       <c r="T33" s="7">
         <f t="shared" si="4"/>
-        <v>14.434448543815277</v>
+        <v>17.484896204741496</v>
       </c>
       <c r="U33" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M33*(proj3!$B$31-proj3!$B$32))</f>
@@ -6362,7 +6358,7 @@
       </c>
       <c r="X33" s="7">
         <f>(R33+ W33+proj3!$B$25/proj3!$B$17 * V33)*(1+proj3!$F$33)</f>
-        <v>0.15640185229617887</v>
+        <v>0.2315093312368704</v>
       </c>
       <c r="Y33" s="7">
         <f>M33 + U33 * proj3!$B$25/proj3!$B$17</f>
@@ -6370,11 +6366,11 @@
       </c>
       <c r="Z33" s="7">
         <f t="shared" si="5"/>
-        <v>8.3460806593081625</v>
+        <v>5.6384011286073825</v>
       </c>
       <c r="AA33" s="7">
         <f t="shared" si="6"/>
-        <v>90.926322164674488</v>
+        <v>41.498883111677046</v>
       </c>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
@@ -6411,19 +6407,19 @@
       </c>
       <c r="Q34" s="7">
         <f t="shared" si="1"/>
-        <v>1.802911038243124E-2</v>
+        <v>1.8051554717825449E-2</v>
       </c>
       <c r="R34" s="7">
         <f t="shared" si="2"/>
-        <v>0.11493230333481108</v>
+        <v>0.19530292128959045</v>
       </c>
       <c r="S34" s="7">
         <f t="shared" si="3"/>
-        <v>3.9505021709720323</v>
+        <v>7.2148938107937415</v>
       </c>
       <c r="T34" s="7">
         <f t="shared" si="4"/>
-        <v>15.836216456686234</v>
+        <v>19.100608096507941</v>
       </c>
       <c r="U34" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M34*(proj3!$B$31-proj3!$B$32))</f>
@@ -6439,7 +6435,7 @@
       </c>
       <c r="X34" s="7">
         <f>(R34+ W34+proj3!$B$25/proj3!$B$17 * V34)*(1+proj3!$F$33)</f>
-        <v>0.17321046365777862</v>
+        <v>0.25920702486939257</v>
       </c>
       <c r="Y34" s="7">
         <f>M34 + U34 * proj3!$B$25/proj3!$B$17</f>
@@ -6447,11 +6443,11 @@
       </c>
       <c r="Z34" s="7">
         <f t="shared" si="5"/>
-        <v>8.0714468519651277</v>
+        <v>5.393600163122283</v>
       </c>
       <c r="AA34" s="7">
         <f t="shared" si="6"/>
-        <v>91.08110659899387</v>
+        <v>40.670827828102169</v>
       </c>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
@@ -6492,19 +6488,19 @@
       </c>
       <c r="Q35" s="7">
         <f t="shared" si="1"/>
-        <v>2.1260033223457549E-2</v>
+        <v>2.1275291925862989E-2</v>
       </c>
       <c r="R35" s="7">
         <f t="shared" si="2"/>
-        <v>0.12741763901749986</v>
+        <v>0.21553036463940345</v>
       </c>
       <c r="S35" s="7">
         <f t="shared" si="3"/>
-        <v>4.1366236516274801</v>
+        <v>7.5548117910201249</v>
       </c>
       <c r="T35" s="7">
         <f t="shared" si="4"/>
-        <v>16.822337937341679</v>
+        <v>20.240526076734326</v>
       </c>
       <c r="U35" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M35*(proj3!$B$31-proj3!$B$32))</f>
@@ -6520,7 +6516,7 @@
       </c>
       <c r="X35" s="7">
         <f>(R35+ W35+proj3!$B$25/proj3!$B$17 * V35)*(1+proj3!$F$33)</f>
-        <v>0.18711424031588814</v>
+        <v>0.28139485673132497</v>
       </c>
       <c r="Y35" s="7">
         <f>M35 + U35 * proj3!$B$25/proj3!$B$17</f>
@@ -6528,11 +6524,11 @@
       </c>
       <c r="Z35" s="7">
         <f t="shared" si="5"/>
-        <v>7.8278895529347192</v>
+        <v>5.2051754747335623</v>
       </c>
       <c r="AA35" s="7">
         <f t="shared" si="6"/>
-        <v>89.75133327865575</v>
+        <v>39.684624908268567</v>
       </c>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
@@ -6569,19 +6565,19 @@
       </c>
       <c r="Q36" s="7">
         <f t="shared" si="1"/>
-        <v>2.6293668426881817E-2</v>
+        <v>2.6299806294444426E-2</v>
       </c>
       <c r="R36" s="7">
         <f t="shared" si="2"/>
-        <v>0.14481154470900584</v>
+        <v>0.2432651698506447</v>
       </c>
       <c r="S36" s="7">
         <f t="shared" si="3"/>
-        <v>4.372870519288834</v>
+        <v>7.9862749290064343</v>
       </c>
       <c r="T36" s="7">
         <f t="shared" si="4"/>
-        <v>18.087156233574532</v>
+        <v>21.700560643292135</v>
       </c>
       <c r="U36" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M36*(proj3!$B$31-proj3!$B$32))</f>
@@ -6597,7 +6593,7 @@
       </c>
       <c r="X36" s="7">
         <f>(R36+ W36+proj3!$B$25/proj3!$B$17 * V36)*(1+proj3!$F$33)</f>
-        <v>0.20641857339970021</v>
+        <v>0.31176395230125381</v>
       </c>
       <c r="Y36" s="7">
         <f>M36 + U36 * proj3!$B$25/proj3!$B$17</f>
@@ -6605,11 +6601,11 @@
       </c>
       <c r="Z36" s="7">
         <f t="shared" si="5"/>
-        <v>7.5056723817808599</v>
+        <v>4.9694975125143879</v>
       </c>
       <c r="AA36" s="7">
         <f t="shared" si="6"/>
-        <v>87.280571965222251</v>
+        <v>38.261617971784048</v>
       </c>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
@@ -6629,7 +6625,7 @@
       </c>
       <c r="H37" s="5">
         <f>H16 / (1+H16/(PI()*H9)*(1+H28))</f>
-        <v>4.4523373266764565</v>
+        <v>3.7667739973868501</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -6653,19 +6649,19 @@
       </c>
       <c r="Q37" s="7">
         <f t="shared" si="1"/>
-        <v>2.8896624166928321E-2</v>
+        <v>2.8898326295462934E-2</v>
       </c>
       <c r="R37" s="7">
         <f t="shared" si="2"/>
-        <v>0.15367372417543224</v>
+        <v>0.25736414944212521</v>
       </c>
       <c r="S37" s="7">
         <f t="shared" si="3"/>
-        <v>4.4877645469941116</v>
+        <v>8.1961085586343359</v>
       </c>
       <c r="T37" s="7">
         <f t="shared" si="4"/>
-        <v>18.887764546994113</v>
+        <v>22.596108558634334</v>
       </c>
       <c r="U37" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M37*(proj3!$B$31-proj3!$B$32))</f>
@@ -6681,7 +6677,7 @@
       </c>
       <c r="X37" s="7">
         <f>(R37+ W37+proj3!$B$25/proj3!$B$17 * V37)*(1+proj3!$F$33)</f>
-        <v>0.2162387701471071</v>
+        <v>0.32718752518246863</v>
       </c>
       <c r="Y37" s="7">
         <f>M37 + U37 * proj3!$B$25/proj3!$B$17</f>
@@ -6689,11 +6685,11 @@
       </c>
       <c r="Z37" s="7">
         <f t="shared" si="5"/>
-        <v>7.3550826034306276</v>
+        <v>4.8609861137255894</v>
       </c>
       <c r="AA37" s="7">
         <f t="shared" si="6"/>
-        <v>86.039172803634656</v>
+        <v>37.581133776789791</v>
       </c>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
@@ -6730,19 +6726,19 @@
       </c>
       <c r="Q38" s="7">
         <f t="shared" si="1"/>
-        <v>2.9195976219513003E-2</v>
+        <v>2.9197196113727807E-2</v>
       </c>
       <c r="R38" s="7">
         <f t="shared" si="2"/>
-        <v>0.15466333475001987</v>
+        <v>0.25893127401310173</v>
       </c>
       <c r="S38" s="7">
         <f t="shared" si="3"/>
-        <v>4.5002553276624919</v>
+        <v>8.2189207612951716</v>
       </c>
       <c r="T38" s="7">
         <f t="shared" si="4"/>
-        <v>19.814541041948193</v>
+        <v>23.533206475580872</v>
       </c>
       <c r="U38" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M38*(proj3!$B$31-proj3!$B$32))</f>
@@ -6758,7 +6754,7 @@
       </c>
       <c r="X38" s="7">
         <f>(R38+ W38+proj3!$B$25/proj3!$B$17 * V38)*(1+proj3!$F$33)</f>
-        <v>0.21733439086000503</v>
+        <v>0.32890108587150263</v>
       </c>
       <c r="Y38" s="7">
         <f>M38 + U38 * proj3!$B$25/proj3!$B$17</f>
@@ -6766,11 +6762,11 @@
       </c>
       <c r="Z38" s="7">
         <f t="shared" si="5"/>
-        <v>7.3385854358002716</v>
+        <v>4.8492603520526956</v>
       </c>
       <c r="AA38" s="7">
         <f t="shared" si="6"/>
-        <v>85.894532089329942</v>
+        <v>37.505228183907946</v>
       </c>
       <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
@@ -6809,19 +6805,19 @@
       </c>
       <c r="Q39" s="7">
         <f t="shared" si="1"/>
-        <v>2.2293694478827605E-2</v>
+        <v>2.2308401534726879E-2</v>
       </c>
       <c r="R39" s="7">
         <f t="shared" si="2"/>
-        <v>0.1291793749685293</v>
+        <v>0.21790121100002766</v>
       </c>
       <c r="S39" s="7">
         <f t="shared" si="3"/>
-        <v>4.1509123391636615</v>
+        <v>7.5809075527252254</v>
       </c>
       <c r="T39" s="7">
         <f t="shared" si="4"/>
-        <v>20.722340910592159</v>
+        <v>24.152336124153724</v>
       </c>
       <c r="U39" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M39*(proj3!$B$31-proj3!$B$32))</f>
@@ -6837,7 +6833,7 @@
       </c>
       <c r="X39" s="7">
         <f>(R39+ W39+proj3!$B$25/proj3!$B$17 * V39)*(1+proj3!$F$33)</f>
-        <v>0.18904114727416652</v>
+        <v>0.28397351182786978</v>
       </c>
       <c r="Y39" s="7">
         <f>M39 + U39 * proj3!$B$25/proj3!$B$17</f>
@@ -6845,11 +6841,11 @@
       </c>
       <c r="Z39" s="7">
         <f t="shared" si="5"/>
-        <v>7.7751666341532788</v>
+        <v>5.1759278930884554</v>
       </c>
       <c r="AA39" s="7">
         <f t="shared" si="6"/>
-        <v>88.855734374781534</v>
+        <v>39.376987217576108</v>
       </c>
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
@@ -6886,19 +6882,19 @@
       </c>
       <c r="Q40" s="7">
         <f t="shared" si="1"/>
-        <v>1.8833966220141132E-2</v>
+        <v>1.8856379455764082E-2</v>
       </c>
       <c r="R40" s="7">
         <f t="shared" si="2"/>
-        <v>0.11577629489982361</v>
+        <v>0.19617965252425495</v>
       </c>
       <c r="S40" s="7">
         <f t="shared" si="3"/>
-        <v>3.951307713849582</v>
+        <v>7.2163649924486393</v>
       </c>
       <c r="T40" s="7">
         <f t="shared" si="4"/>
-        <v>20.979879142420984</v>
+        <v>24.244936421020039</v>
       </c>
       <c r="U40" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M40*(proj3!$B$31-proj3!$B$32))</f>
@@ -6914,7 +6910,7 @@
       </c>
       <c r="X40" s="7">
         <f>(R40+ W40+proj3!$B$25/proj3!$B$17 * V40)*(1+proj3!$F$33)</f>
-        <v>0.17411588849163667</v>
+        <v>0.2601474811497782</v>
       </c>
       <c r="Y40" s="7">
         <f>M40 + U40 * proj3!$B$25/proj3!$B$17</f>
@@ -6922,11 +6918,11 @@
       </c>
       <c r="Z40" s="7">
         <f t="shared" si="5"/>
-        <v>8.0311310506898295</v>
+        <v>5.3752106778175648</v>
       </c>
       <c r="AA40" s="7">
         <f t="shared" si="6"/>
-        <v>90.192108820385116</v>
+        <v>40.402300796893471</v>
       </c>
       <c r="AB40" s="2"/>
       <c r="AC40" s="2"/>
@@ -6963,19 +6959,19 @@
       </c>
       <c r="Q41" s="7">
         <f t="shared" si="1"/>
-        <v>1.371787326841614E-2</v>
+        <v>1.3755073525558145E-2</v>
       </c>
       <c r="R41" s="7">
         <f t="shared" si="2"/>
-        <v>9.2952374122571915E-2</v>
+        <v>0.15854265730656741</v>
       </c>
       <c r="S41" s="7">
         <f t="shared" si="3"/>
-        <v>3.5682958979230839</v>
+        <v>6.5168616228532183</v>
       </c>
       <c r="T41" s="7">
         <f t="shared" si="4"/>
-        <v>21.625438755065883</v>
+        <v>24.57400447999602</v>
       </c>
       <c r="U41" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M41*(proj3!$B$31-proj3!$B$32))</f>
@@ -6991,7 +6987,7 @@
       </c>
       <c r="X41" s="7">
         <f>(R41+ W41+proj3!$B$25/proj3!$B$17 * V41)*(1+proj3!$F$33)</f>
-        <v>0.14857767459261742</v>
+        <v>0.21875927759949257</v>
       </c>
       <c r="Y41" s="7">
         <f>M41 + U41 * proj3!$B$25/proj3!$B$17</f>
@@ -6999,11 +6995,11 @@
       </c>
       <c r="Z41" s="7">
         <f t="shared" si="5"/>
-        <v>8.4884223566813173</v>
+        <v>5.7651957373195355</v>
       </c>
       <c r="AA41" s="7">
         <f t="shared" si="6"/>
-        <v>90.87292315904574</v>
+        <v>41.918781602965836</v>
       </c>
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
@@ -7040,19 +7036,19 @@
       </c>
       <c r="Q42" s="7">
         <f t="shared" si="1"/>
-        <v>1.3307461905549108E-2</v>
+        <v>1.3349349616992677E-2</v>
       </c>
       <c r="R42" s="7">
         <f t="shared" si="2"/>
-        <v>8.7305170192193832E-2</v>
+        <v>0.14851504992825651</v>
       </c>
       <c r="S42" s="7">
         <f t="shared" si="3"/>
-        <v>3.4468819687013039</v>
+        <v>6.295120545750903</v>
       </c>
       <c r="T42" s="7">
         <f t="shared" si="4"/>
-        <v>22.189739111558406</v>
+        <v>25.037977688608002</v>
       </c>
       <c r="U42" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M42*(proj3!$B$31-proj3!$B$32))</f>
@@ -7068,7 +7064,7 @@
       </c>
       <c r="X42" s="7">
         <f>(R42+ W42+proj3!$B$25/proj3!$B$17 * V42)*(1+proj3!$F$33)</f>
-        <v>0.14218227660881241</v>
+        <v>0.20767684792639948</v>
       </c>
       <c r="Y42" s="7">
         <f>M42 + U42 * proj3!$B$25/proj3!$B$17</f>
@@ -7076,11 +7072,11 @@
       </c>
       <c r="Z42" s="7">
         <f t="shared" si="5"/>
-        <v>8.564438973051681</v>
+        <v>5.8634914927892376</v>
       </c>
       <c r="AA42" s="7">
         <f t="shared" si="6"/>
-        <v>89.318664556160471</v>
+        <v>41.865567414343111</v>
       </c>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
@@ -7117,19 +7113,19 @@
       </c>
       <c r="Q43" s="7">
         <f t="shared" si="1"/>
-        <v>1.3015486839961414E-2</v>
+        <v>1.3061466332184067E-2</v>
       </c>
       <c r="R43" s="7">
         <f t="shared" si="2"/>
-        <v>8.259006521891743E-2</v>
+        <v>0.14010027599527511</v>
       </c>
       <c r="S43" s="7">
         <f t="shared" si="3"/>
-        <v>3.3408971099824667</v>
+        <v>6.1015579382355547</v>
       </c>
       <c r="T43" s="7">
         <f t="shared" si="4"/>
-        <v>22.769468538553866</v>
+        <v>25.530129366806953</v>
       </c>
       <c r="U43" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M43*(proj3!$B$31-proj3!$B$32))</f>
@@ -7145,7 +7141,7 @@
       </c>
       <c r="X43" s="7">
         <f>(R43+ W43+proj3!$B$25/proj3!$B$17 * V43)*(1+proj3!$F$33)</f>
-        <v>0.13682949253788307</v>
+        <v>0.19836541806858579</v>
       </c>
       <c r="Y43" s="7">
         <f>M43 + U43 * proj3!$B$25/proj3!$B$17</f>
@@ -7153,11 +7149,11 @@
       </c>
       <c r="Z43" s="7">
         <f t="shared" si="5"/>
-        <v>8.6221031244416224</v>
+        <v>5.9473975182445171</v>
       </c>
       <c r="AA43" s="7">
         <f t="shared" si="6"/>
-        <v>87.703990697874687</v>
+        <v>41.72985385883463</v>
       </c>
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
@@ -7194,19 +7190,19 @@
       </c>
       <c r="Q44" s="7">
         <f t="shared" si="1"/>
-        <v>1.2030326543704676E-2</v>
+        <v>1.2080201457330566E-2</v>
       </c>
       <c r="R44" s="7">
         <f t="shared" si="2"/>
-        <v>7.7522377837309378E-2</v>
+        <v>0.13161793114237708</v>
       </c>
       <c r="S44" s="7">
         <f t="shared" si="3"/>
-        <v>3.2399983303647732</v>
+        <v>5.9172841550366924</v>
       </c>
       <c r="T44" s="7">
         <f t="shared" si="4"/>
-        <v>23.582855473221873</v>
+        <v>26.260141297893792</v>
       </c>
       <c r="U44" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M44*(proj3!$B$31-proj3!$B$32))</f>
@@ -7222,7 +7218,7 @@
       </c>
       <c r="X44" s="7">
         <f>(R44+ W44+proj3!$B$25/proj3!$B$17 * V44)*(1+proj3!$F$33)</f>
-        <v>0.13111457439437832</v>
+        <v>0.18899681643080077</v>
       </c>
       <c r="Y44" s="7">
         <f>M44 + U44 * proj3!$B$25/proj3!$B$17</f>
@@ -7230,11 +7226,11 @@
       </c>
       <c r="Z44" s="7">
         <f t="shared" si="5"/>
-        <v>8.722339997507822</v>
+        <v>6.0510325945888495</v>
       </c>
       <c r="AA44" s="7">
         <f t="shared" si="6"/>
-        <v>87.006160495848519</v>
+        <v>41.873857009038709</v>
       </c>
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
@@ -7271,19 +7267,19 @@
       </c>
       <c r="Q45" s="7">
         <f t="shared" si="1"/>
-        <v>1.2965100382879942E-2</v>
+        <v>1.3011352951877395E-2</v>
       </c>
       <c r="R45" s="7">
         <f t="shared" si="2"/>
-        <v>8.2249405173945772E-2</v>
+        <v>0.13951682496582193</v>
       </c>
       <c r="S45" s="7">
         <f t="shared" si="3"/>
-        <v>3.3338239051948317</v>
+        <v>6.0886399801542339</v>
       </c>
       <c r="T45" s="7">
         <f t="shared" si="4"/>
-        <v>23.790966762337632</v>
+        <v>26.545782837297033</v>
       </c>
       <c r="U45" s="9">
         <f>1/proj3!$B$35*(proj3!$B$27+M45*(proj3!$B$31-proj3!$B$32))</f>
@@ -7299,7 +7295,7 @@
       </c>
       <c r="X45" s="7">
         <f>(R45+ W45+proj3!$B$25/proj3!$B$17 * V45)*(1+proj3!$F$33)</f>
-        <v>0.13644447031542101</v>
+        <v>0.19772060949272852</v>
       </c>
       <c r="Y45" s="7">
         <f>M45 + U45 * proj3!$B$25/proj3!$B$17</f>
@@ -7307,11 +7303,11 @@
       </c>
       <c r="Z45" s="7">
         <f t="shared" si="5"/>
-        <v>8.6278693489760343</v>
+        <v>5.9539825731469103</v>
       </c>
       <c r="AA45" s="7">
         <f t="shared" si="6"/>
-        <v>87.632786164122194</v>
+        <v>41.732520754917736</v>
       </c>
       <c r="AB45" s="2"/>
       <c r="AC45" s="2"/>
@@ -7592,10 +7588,10 @@
       <c r="F54" s="2"/>
       <c r="G54" s="5">
         <f t="array" ref="G54:H54">LINEST(O3:O45,T3:T45)</f>
-        <v>6.2270180372468419E-2</v>
+        <v>5.4655027077242943E-2</v>
       </c>
       <c r="H54" s="5">
-        <v>0.15428215469597839</v>
+        <v>0.13346740254162603</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -7629,7 +7625,7 @@
       <c r="F55" s="2"/>
       <c r="G55" s="5">
         <f>180/PI() *G54</f>
-        <v>3.567818524860817</v>
+        <v>3.1315023806992559</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -7696,7 +7692,7 @@
       <c r="F57" s="2"/>
       <c r="G57" s="5">
         <f>G52/(1+G52/(PI() * H9) * (1+H28))</f>
-        <v>3.5284243416212155</v>
+        <v>3.0836534748776518</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -37915,9 +37911,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="E18" sqref="E18:E19"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -40319,9 +40312,8 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:B30"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -41136,7 +41128,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -55721,9 +55712,6 @@
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:D1"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -56288,9 +56276,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
-    <sheetView topLeftCell="A4" workbookViewId="1">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -71891,7 +71876,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
@@ -73580,9 +73564,6 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:B1"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
@@ -73722,11 +73703,11 @@
       </c>
       <c r="G8" s="87">
         <f xml:space="preserve"> E8/(F8*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-0.16442302973386907</v>
+        <v>-0.13398601185628983</v>
       </c>
       <c r="H8" s="87">
         <f xml:space="preserve"> DEGREES(G8)</f>
-        <v>-9.4207456585047407</v>
+        <v>-7.6768329931552159</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -73747,11 +73728,11 @@
       </c>
       <c r="G9" s="87">
         <f xml:space="preserve"> E9/(F9*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-0.13307209685962312</v>
+        <v>-0.10263507898204391</v>
       </c>
       <c r="H9" s="87">
         <f xml:space="preserve"> DEGREES(G9)</f>
-        <v>-7.6244695210125011</v>
+        <v>-5.8805568556629773</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -73773,11 +73754,11 @@
       </c>
       <c r="G10" s="87">
         <f xml:space="preserve"> E10/(F10*$B$33)-$B$36/$B$31*(1-$B$37)</f>
-        <v>-9.8444589909657404E-2</v>
+        <v>-6.800757203207819E-2</v>
       </c>
       <c r="H10" s="87">
         <f t="shared" ref="H10" si="0" xml:space="preserve"> DEGREES(G10)</f>
-        <v>-5.6404595177195391</v>
+        <v>-3.8965468523700157</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -73908,7 +73889,7 @@
       </c>
       <c r="B25" s="91">
         <f>proj2_copy!H9</f>
-        <v>6.5967841001666665</v>
+        <v>3.5594158813848917</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="127" t="s">
@@ -74004,7 +73985,7 @@
       </c>
       <c r="B31" s="84">
         <f>proj2_copy!H37</f>
-        <v>4.4523373266764565</v>
+        <v>3.7667739973868501</v>
       </c>
       <c r="M31">
         <v>0.1</v>
@@ -74113,7 +74094,7 @@
       </c>
       <c r="B37" s="84">
         <f xml:space="preserve"> 2*B31/(PI()*B25)</f>
-        <v>0.42967087180264696</v>
+        <v>0.67370683412344901</v>
       </c>
       <c r="F37" s="80" t="s">
         <v>339</v>

</xml_diff>